<commit_message>
Added SOFIA tables, scripts, images
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="15340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="19660" windowHeight="15340" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
     <sheet name="FORCAST Sensitivity" sheetId="2" r:id="rId2"/>
     <sheet name="Starcamera" sheetId="3" r:id="rId3"/>
+    <sheet name="TotalFluxTables" sheetId="4" r:id="rId4"/>
+    <sheet name="CompareGuthMegeath" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="124">
   <si>
     <t>\toprule</t>
   </si>
@@ -303,6 +305,96 @@
   </si>
   <si>
     <t xml:space="preserve">  Fit ra \&amp; dec error (arcsec) </t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F19</t>
+  </si>
+  <si>
+    <t>F31</t>
+  </si>
+  <si>
+    <t>F37</t>
+  </si>
+  <si>
+    <t>NGC2071.1</t>
+  </si>
+  <si>
+    <t>NGC2071.2</t>
+  </si>
+  <si>
+    <t>NGC2071.3</t>
+  </si>
+  <si>
+    <t>Error (%)</t>
+  </si>
+  <si>
+    <t>IRAS20050.1</t>
+  </si>
+  <si>
+    <t>IRAS20050.2</t>
+  </si>
+  <si>
+    <t>IRAS20050.3</t>
+  </si>
+  <si>
+    <t>IRAS20050.4</t>
+  </si>
+  <si>
+    <t>IRAS20050.5</t>
+  </si>
+  <si>
+    <t>SOFIA name</t>
+  </si>
+  <si>
+    <t>S140.3</t>
+  </si>
+  <si>
+    <t>S140.4</t>
+  </si>
+  <si>
+    <t>S140.5</t>
+  </si>
+  <si>
+    <t>Sum of point sources in cluster</t>
+  </si>
+  <si>
+    <t>Total cluster emission</t>
+  </si>
+  <si>
+    <t>F11L</t>
+  </si>
+  <si>
+    <t>F31L</t>
+  </si>
+  <si>
+    <t>F37L</t>
+  </si>
+  <si>
+    <t>i1</t>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>NGC2071.4</t>
+  </si>
+  <si>
+    <t>NGC2071.5</t>
+  </si>
+  <si>
+    <t>IRAS20050.6</t>
+  </si>
+  <si>
+    <t>IRAS20050.7</t>
   </si>
 </sst>
 </file>
@@ -358,7 +450,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -480,16 +572,95 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="197">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -550,6 +721,44 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -610,6 +819,44 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -942,11 +1189,12 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="3" max="3" width="35" customWidth="1"/>
     <col min="5" max="5" width="25.5" customWidth="1"/>
     <col min="9" max="9" width="24.5" customWidth="1"/>
     <col min="11" max="11" width="35.33203125" customWidth="1"/>
@@ -1795,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -4094,13 +4342,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -4198,13 +4448,13 @@
       <c r="F6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>259.67796600000003</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>92.190746000000004</v>
       </c>
       <c r="J6" s="5" t="s">
@@ -4234,13 +4484,13 @@
       <c r="R6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="6">
         <v>113.923585</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="4">
         <v>40.310223999999998</v>
       </c>
       <c r="V6" s="5" t="s">
@@ -4258,7 +4508,7 @@
       <c r="Z6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA6" s="5">
+      <c r="AA6" s="4">
         <v>98.333332999999996</v>
       </c>
       <c r="AB6" t="s">
@@ -4284,13 +4534,13 @@
       <c r="F7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>113.25</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>13.195906000000001</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -4320,13 +4570,13 @@
       <c r="R7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="6">
         <v>117.703881</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="4">
         <v>32.179909000000002</v>
       </c>
       <c r="V7" s="5" t="s">
@@ -4344,7 +4594,7 @@
       <c r="Z7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AA7" s="4">
         <v>100</v>
       </c>
       <c r="AB7" t="s">
@@ -4370,13 +4620,13 @@
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>69.653060999999994</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>52.944156999999997</v>
       </c>
       <c r="J8" s="5" t="s">
@@ -4406,13 +4656,13 @@
       <c r="R8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="6">
         <v>155.38567599999999</v>
       </c>
       <c r="T8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="4">
         <v>66.113045999999997</v>
       </c>
       <c r="V8" s="5" t="s">
@@ -4430,7 +4680,7 @@
       <c r="Z8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA8" s="5">
+      <c r="AA8" s="4">
         <v>96.078430999999995</v>
       </c>
       <c r="AB8" t="s">
@@ -4456,13 +4706,13 @@
       <c r="F9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>66.136364</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>23.349055</v>
       </c>
       <c r="J9" s="5" t="s">
@@ -4492,13 +4742,13 @@
       <c r="R9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="6">
         <v>151.262461</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="4">
         <v>55.189838000000002</v>
       </c>
       <c r="V9" s="5" t="s">
@@ -4516,7 +4766,7 @@
       <c r="Z9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA9" s="5">
+      <c r="AA9" s="4">
         <v>75.862069000000005</v>
       </c>
       <c r="AB9" t="s">
@@ -4542,13 +4792,13 @@
       <c r="F10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>44.314286000000003</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>52.523068000000002</v>
       </c>
       <c r="J10" s="5" t="s">
@@ -4578,13 +4828,13 @@
       <c r="R10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="6">
         <v>179.73397</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="4">
         <v>65.379571999999996</v>
       </c>
       <c r="V10" s="5" t="s">
@@ -4602,7 +4852,7 @@
       <c r="Z10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AA10" s="4">
         <v>36.842104999999997</v>
       </c>
       <c r="AB10" t="s">
@@ -4846,6 +5096,1374 @@
       <c r="N20" t="s">
         <v>91</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="2.5" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="2.5" customWidth="1"/>
+    <col min="13" max="13" width="7.5" customWidth="1"/>
+    <col min="14" max="14" width="3" customWidth="1"/>
+    <col min="15" max="15" width="8.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>9.9098232236099992</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>70.911149322399993</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>173.25481492599999</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>240.80440230400001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.21512971776100001</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>11.077599559499999</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>54.873213537600002</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5">
+        <v>83.371307746599996</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.40490885879900002</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.2212143580700001</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>20.6188733625</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5">
+        <v>38.067091976</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <f>SUM(C3:C5)</f>
+        <v>10.52986180017</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" ref="E7:I7" si="0">SUM(E3:E5)</f>
+        <v>85.209963239969994</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>248.74690182610001</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>362.24280202659997</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>11.329523011499999</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>94.039490667500004</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>277.78013015300002</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>357.18574971999999</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" ref="C9:G9" si="1">(C8-C7)/C7*100</f>
+        <v>7.5942232339373072</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>10.362083366547314</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="1"/>
+        <v>11.671794950514499</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <f>(I8-I7)/I7*100</f>
+        <v>-1.3960394183977849</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.614573017</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.0768330289999999</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5.3738602850000001</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>7.7896056939999996</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.9632009999999997E-2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.416479233</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <v>9.3476763569999992</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>12.37225617</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.19636084000000001</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.4097560869999999</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2">
+        <v>12.41054997</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>19.448379490000001</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4.0852307999999997E-2</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.14858833499999999</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7.8177788110000002</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>12.330035049999999</v>
+      </c>
+      <c r="J18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.20614339700000001</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.6606400859999999</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6.1319755020000004</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>10.311542640000001</v>
+      </c>
+      <c r="J19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <f>SUM(C15:C19)</f>
+        <v>1.1075615719999998</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <f>SUM(E15:E19)</f>
+        <v>7.71229677</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
+        <f>SUM(G15:G19)</f>
+        <v>41.081840925000009</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <f>SUM(I15:I19)</f>
+        <v>62.251819043999994</v>
+      </c>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.6511213220000001</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7.0253575079999999</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>37.873027069999999</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2">
+        <v>49.35974126</v>
+      </c>
+      <c r="J22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <f>(C22-C21)/C21*100</f>
+        <v>49.077158664728422</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <f>(E22-E21)/E21*100</f>
+        <v>-8.9070646849602504</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <f>(G22-G21)/G21*100</f>
+        <v>-7.8107839930009391</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
+        <f>(I22-I21)/I21*100</f>
+        <v>-20.709559948582047</v>
+      </c>
+      <c r="J23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>9.7880270849999995</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <v>101.7042635</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2">
+        <v>449.60469970000003</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>401</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2">
+        <v>639.16812279999999</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" s="2">
+        <v>669</v>
+      </c>
+      <c r="P27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.6177842120000001</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>91.090846869999993</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>357.63365320000003</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" s="2">
+        <v>368</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
+        <v>367.35382920000001</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="2">
+        <v>485</v>
+      </c>
+      <c r="P28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>110.0219116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>110</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>812.83911339999997</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1857.3335959999999</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1585</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="2">
+        <v>2000.9436270000001</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2">
+        <v>2176</v>
+      </c>
+      <c r="P29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <f>SUM(C27:C29)</f>
+        <v>123.427722897</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f>SUM(E27:E29)</f>
+        <v>123.7</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <f>SUM(G27:G29)</f>
+        <v>1005.6342237699999</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" ref="I31" si="2">SUM(I27:I29)</f>
+        <v>2664.5719489000003</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f>SUM(K27:K29)</f>
+        <v>2354</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" ref="M31" si="3">SUM(M27:M29)</f>
+        <v>3007.4655790000002</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <f>SUM(O27:O29)</f>
+        <v>3330</v>
+      </c>
+      <c r="P31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>135.26027999999999</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>145</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1195.2043180000001</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2">
+        <v>4450.3103659999997</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" s="2">
+        <v>3780</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M32" s="2">
+        <v>5910.258425</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O32" s="2">
+        <v>6730</v>
+      </c>
+      <c r="P32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5">
+        <f>(C32-C31)/C31*100</f>
+        <v>9.5866283726827142</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" ref="E33" si="4">(E32-E31)/E31*100</f>
+        <v>17.21907841552142</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" ref="G33" si="5">(G32-G31)/G31*100</f>
+        <v>18.850799798690719</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" ref="I33" si="6">(I32-I31)/I31*100</f>
+        <v>67.017834434427471</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" ref="K33:O33" si="7">(K32-K31)/K31*100</f>
+        <v>60.577740016992351</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M33" s="5">
+        <f t="shared" si="7"/>
+        <v>96.51957004160279</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" si="7"/>
+        <v>102.10210210210211</v>
+      </c>
+      <c r="P33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.3064506000000002E-2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.0707374000000001E-2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.8922937000000001E-2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>-3.3639657000000003E-2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-6.7145516000000002E-2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-9.7067649000000006E-2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-6.4755173999999999E-2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>-8.9613622000000004E-2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.1372058000000003E-2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>-0.116380185</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-6.3361789999999999E-3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>-0.103188105</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-5.2550110999999997E-2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>-5.5211809000000001E-2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-0.114044351</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2">
+        <v>-0.11330852900000001</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-8.0717134999999995E-2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>-6.2221011E-2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-6.6484915000000006E-2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8.2687483000000006E-2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.193836708</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.10340400900000001</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.7424160999999999E-2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>9.9953852999999995E-2</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-7.1202603000000003E-2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>-5.5787059999999999E-2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-0.11777913700000001</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>-4.6784953999999997E-2</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-0.150915566</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>-7.2107030000000003E-2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-1.8941323999999999E-2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>-7.3121799000000001E-2</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated a bunch of references, improved the SOFIA section
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="2060" windowWidth="21260" windowHeight="15620" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="15380" yWindow="1440" windowWidth="21260" windowHeight="15620" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="TotalFluxTables" sheetId="4" r:id="rId4"/>
     <sheet name="CompareGuthMegeath" sheetId="5" r:id="rId5"/>
     <sheet name="grid" sheetId="6" r:id="rId6"/>
+    <sheet name="Hyperion params" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="213">
   <si>
     <t>\toprule</t>
   </si>
@@ -329,9 +330,6 @@
     <t>NGC2071.3</t>
   </si>
   <si>
-    <t>Error (%)</t>
-  </si>
-  <si>
     <t>IRAS20050.1</t>
   </si>
   <si>
@@ -627,6 +625,45 @@
   </si>
   <si>
     <t>\multicolumn{4}{c}{Central source}</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Number of photons (initial)</t>
+  </si>
+  <si>
+    <t>\num{2e5}</t>
+  </si>
+  <si>
+    <t>Number of photons (imaging)</t>
+  </si>
+  <si>
+    <t>Number of photons (raytracing sources)</t>
+  </si>
+  <si>
+    <t>\num{1e6}</t>
+  </si>
+  <si>
+    <t>Number of photons (raytracing dust)</t>
+  </si>
+  <si>
+    <t>Lucy max iterations</t>
+  </si>
+  <si>
+    <t>Max photon interactions</t>
+  </si>
+  <si>
+    <t>\num{1e5}</t>
+  </si>
+  <si>
+    <t>Geometrical grid parameters (radial, theta and azimuthal)</t>
+  </si>
+  <si>
+    <t>400, 199, 2</t>
+  </si>
+  <si>
+    <t>MRW</t>
   </si>
 </sst>
 </file>
@@ -682,8 +719,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="307">
+  <cellStyleXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1003,7 +1048,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="307">
+  <cellStyles count="315">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1157,6 +1202,10 @@
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1310,6 +1359,10 @@
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5566,7 +5619,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:P33"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5590,7 +5643,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5735,7 +5788,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -5771,7 +5824,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -5803,35 +5856,35 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" ref="C9:G9" si="1">(C8-C7)/C7*100</f>
-        <v>7.5942232339373072</v>
+        <f>(C8)/C7</f>
+        <v>1.075942232339373</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>10.362083366547314</v>
+        <f>(E8)/E7</f>
+        <v>1.1036208336654731</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="1"/>
-        <v>11.671794950514499</v>
+        <f>(G8)/G7</f>
+        <v>1.1167179495051449</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="5">
-        <f>(I8-I7)/I7*100</f>
-        <v>-1.3960394183977849</v>
+        <f>(I8)/I7</f>
+        <v>0.98603960581602212</v>
       </c>
       <c r="J9" t="s">
         <v>40</v>
@@ -5866,7 +5919,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -5910,7 +5963,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -5942,7 +5995,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
@@ -5966,7 +6019,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="2">
-        <v>12.37225617</v>
+        <v>12</v>
       </c>
       <c r="J16" t="s">
         <v>40</v>
@@ -5974,7 +6027,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -6006,7 +6059,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -6038,7 +6091,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
@@ -6082,7 +6135,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
@@ -6110,7 +6163,7 @@
       </c>
       <c r="I21" s="5">
         <f>SUM(I15:I19)</f>
-        <v>62.251819043999994</v>
+        <v>61.879562873999994</v>
       </c>
       <c r="J21" t="s">
         <v>40</v>
@@ -6118,7 +6171,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -6150,35 +6203,35 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <f>(C22-C21)/C21*100</f>
-        <v>49.077158664728422</v>
+        <f t="shared" ref="C23:H23" si="1">(C22)/C21</f>
+        <v>1.4907715866472842</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <f>(E22-E21)/E21*100</f>
-        <v>-8.9070646849602504</v>
+        <f t="shared" si="1"/>
+        <v>0.91092935315039747</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="5">
-        <f>(G22-G21)/G21*100</f>
-        <v>-7.8107839930009391</v>
+        <f t="shared" si="1"/>
+        <v>0.92189216006999064</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="5">
-        <f>(I22-I21)/I21*100</f>
-        <v>-20.709559948582047</v>
+        <f>(I22)/I21</f>
+        <v>0.79767436884625342</v>
       </c>
       <c r="J23" t="s">
         <v>40</v>
@@ -6186,7 +6239,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -6198,7 +6251,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>1</v>
@@ -6216,7 +6269,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>1</v>
@@ -6228,7 +6281,7 @@
         <v>1</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P25" t="s">
         <v>40</v>
@@ -6248,7 +6301,7 @@
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>1</v>
@@ -6298,7 +6351,7 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>1</v>
@@ -6348,7 +6401,7 @@
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>1</v>
@@ -6410,7 +6463,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1</v>
@@ -6467,7 +6520,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
@@ -6517,56 +6570,56 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="5">
-        <f>(C32-C31)/C31*100</f>
-        <v>9.5866283726827142</v>
+        <f>(C32)/C31</f>
+        <v>1.0958662837268272</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" ref="E33" si="4">(E32-E31)/E31*100</f>
-        <v>17.21907841552142</v>
+        <f>(E32)/E31</f>
+        <v>1.1721907841552142</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="5">
-        <f t="shared" ref="G33" si="5">(G32-G31)/G31*100</f>
-        <v>18.850799798690719</v>
+        <f>(G32)/G31</f>
+        <v>1.1885079979869071</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="I33" s="5">
-        <f t="shared" ref="I33" si="6">(I32-I31)/I31*100</f>
-        <v>67.017834434427471</v>
+        <f>(I32)/I31</f>
+        <v>1.6701783443442746</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" ref="K33:O33" si="7">(K32-K31)/K31*100</f>
-        <v>60.577740016992351</v>
+        <f>(K32)/K31</f>
+        <v>1.6057774001699234</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" si="7"/>
-        <v>96.51957004160279</v>
+        <f>(M32)/M31</f>
+        <v>1.9651957004160279</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="7"/>
-        <v>102.10210210210211</v>
+        <f>(O32)/O31</f>
+        <v>2.0210210210210211</v>
       </c>
       <c r="P33" t="s">
         <v>40</v>
@@ -6591,7 +6644,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6603,31 +6656,31 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>40</v>
@@ -6713,7 +6766,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -6745,7 +6798,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -6791,7 +6844,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
@@ -6823,7 +6876,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -6855,7 +6908,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
@@ -6887,7 +6940,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -6935,7 +6988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -6947,25 +7000,25 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>124</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>125</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>126</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>127</v>
       </c>
       <c r="H3" t="s">
         <v>40</v>
@@ -6978,7 +7031,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -6991,7 +7044,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
@@ -6999,14 +7052,14 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
         <v>128</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>129</v>
-      </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
@@ -7017,7 +7070,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H8" t="s">
         <v>40</v>
@@ -7025,13 +7078,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>130</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>131</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -7043,7 +7096,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
         <v>40</v>
@@ -7056,7 +7109,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" t="s">
         <v>40</v>
@@ -7064,19 +7117,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>145</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>146</v>
       </c>
       <c r="F12" t="s">
         <v>1</v>
@@ -7087,13 +7140,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -7105,7 +7158,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H13" t="s">
         <v>40</v>
@@ -7113,13 +7166,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -7131,7 +7184,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H14" t="s">
         <v>40</v>
@@ -7139,25 +7192,25 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F15" t="s">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H15" t="s">
         <v>40</v>
@@ -7165,13 +7218,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -7188,13 +7241,13 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -7211,25 +7264,25 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>141</v>
       </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>142</v>
-      </c>
       <c r="D18" t="s">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" t="s">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H18" t="s">
         <v>40</v>
@@ -7237,25 +7290,25 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>139</v>
       </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>140</v>
-      </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F19" t="s">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H19" t="s">
         <v>40</v>
@@ -7263,19 +7316,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>143</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>144</v>
       </c>
       <c r="F20" t="s">
         <v>1</v>
@@ -7291,7 +7344,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H22" t="s">
         <v>40</v>
@@ -7299,19 +7352,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
         <v>1</v>
@@ -7322,25 +7375,25 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F24" t="s">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H24" t="s">
         <v>40</v>
@@ -7348,13 +7401,13 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -7366,7 +7419,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H25" t="s">
         <v>40</v>
@@ -7374,13 +7427,13 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -7397,25 +7450,25 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H27" t="s">
         <v>40</v>
@@ -7423,19 +7476,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>143</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>144</v>
       </c>
       <c r="F28" t="s">
         <v>1</v>
@@ -7451,7 +7504,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H30" t="s">
         <v>40</v>
@@ -7459,25 +7512,25 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="s">
         <v>167</v>
       </c>
-      <c r="D31" t="s">
-        <v>168</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F31" t="s">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H31" t="s">
         <v>40</v>
@@ -7485,13 +7538,13 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
@@ -7503,7 +7556,7 @@
         <v>1</v>
       </c>
       <c r="G32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H32" t="s">
         <v>40</v>
@@ -7514,7 +7567,7 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
@@ -7531,13 +7584,13 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -7549,7 +7602,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" t="s">
         <v>40</v>
@@ -7557,13 +7610,13 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -7590,7 +7643,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H38" t="s">
         <v>40</v>
@@ -7603,25 +7656,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F40" t="s">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H40" t="s">
         <v>40</v>
@@ -7629,25 +7682,25 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F41" t="s">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H41" t="s">
         <v>40</v>
@@ -7655,25 +7708,25 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F42" t="s">
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H42" t="s">
         <v>40</v>
@@ -7681,19 +7734,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F43" t="s">
         <v>1</v>
@@ -7704,24 +7757,160 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F44" t="s">
         <v>1</v>
       </c>
       <c r="H44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Heavily edited the IRAS20050 section, added new data
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="1440" windowWidth="21260" windowHeight="15620" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="12860" yWindow="820" windowWidth="21260" windowHeight="17080" tabRatio="652" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="CompareGuthMegeath" sheetId="5" r:id="rId5"/>
     <sheet name="grid" sheetId="6" r:id="rId6"/>
     <sheet name="Hyperion params" sheetId="7" r:id="rId7"/>
+    <sheet name="IRAS20050" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="222">
   <si>
     <t>\toprule</t>
   </si>
@@ -664,12 +665,42 @@
   </si>
   <si>
     <t>MRW</t>
+  </si>
+  <si>
+    <t>Coordinates</t>
+  </si>
+  <si>
+    <t>ks</t>
+  </si>
+  <si>
+    <t>20h07m06.638s +27d28m47.971s</t>
+  </si>
+  <si>
+    <t>20h07m06.197s +27d28m49.127s</t>
+  </si>
+  <si>
+    <t>20h07m06.319s +27d28m56.568s</t>
+  </si>
+  <si>
+    <t>20h07m05.858s +27d28m59.182s</t>
+  </si>
+  <si>
+    <t>20h07m06.571s +27d28m53.137s</t>
+  </si>
+  <si>
+    <t>20h07m02.172s +27d30m26.014s</t>
+  </si>
+  <si>
+    <t>20h07m07.927s +27d27m15.782s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -719,7 +750,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="315">
+  <cellStyleXfs count="369">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1035,20 +1066,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="315">
+  <cellStyles count="369">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1206,6 +1292,33 @@
     <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1363,6 +1476,33 @@
     <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4990,7 +5130,7 @@
       <c r="R6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="7">
         <v>113.923585</v>
       </c>
       <c r="T6" s="5" t="s">
@@ -5076,7 +5216,7 @@
       <c r="R7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="7">
         <v>117.703881</v>
       </c>
       <c r="T7" s="5" t="s">
@@ -5162,7 +5302,7 @@
       <c r="R8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="7">
         <v>155.38567599999999</v>
       </c>
       <c r="T8" s="5" t="s">
@@ -5248,7 +5388,7 @@
       <c r="R9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="7">
         <v>151.262461</v>
       </c>
       <c r="T9" s="5" t="s">
@@ -5334,7 +5474,7 @@
       <c r="R10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="7">
         <v>179.73397</v>
       </c>
       <c r="T10" s="5" t="s">
@@ -5618,8 +5758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5628,7 +5768,7 @@
     <col min="2" max="2" width="2.6640625" customWidth="1"/>
     <col min="3" max="3" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="2.83203125" customWidth="1"/>
-    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" customWidth="1"/>
     <col min="8" max="8" width="2.5" customWidth="1"/>
@@ -5686,25 +5826,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>9.9098232236099992</v>
+        <v>10.071999999999999</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5">
-        <v>70.911149322399993</v>
+      <c r="E3">
+        <v>72.040999999999997</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="5">
-        <v>173.25481492599999</v>
+        <v>167.929</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I3" s="5">
-        <v>240.80440230400001</v>
+        <v>234.93</v>
       </c>
       <c r="J3" t="s">
         <v>40</v>
@@ -5718,25 +5858,25 @@
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0.21512971776100001</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>11.077599559499999</v>
+      <c r="E4">
+        <v>11.207000000000001</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>54.873213537600002</v>
+        <v>56.703000000000003</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>83.371307746599996</v>
+        <v>89.546000000000006</v>
       </c>
       <c r="J4" t="s">
         <v>40</v>
@@ -5750,25 +5890,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0.40490885879900002</v>
+        <v>0.192</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
-        <v>3.2212143580700001</v>
+      <c r="E5">
+        <v>3.0270000000000001</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="5">
-        <v>20.6188733625</v>
+        <v>19.974</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>38.067091976</v>
+        <v>37.555999999999997</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
@@ -5795,28 +5935,28 @@
       </c>
       <c r="C7" s="5">
         <f>SUM(C3:C5)</f>
-        <v>10.52986180017</v>
+        <v>10.646999999999998</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" ref="E7:I7" si="0">SUM(E3:E5)</f>
-        <v>85.209963239969994</v>
+        <v>86.274999999999991</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
-        <v>248.74690182610001</v>
+        <v>244.60599999999999</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>362.24280202659997</v>
+        <v>362.03199999999998</v>
       </c>
       <c r="J7" t="s">
         <v>40</v>
@@ -5829,26 +5969,26 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
-        <v>11.329523011499999</v>
+      <c r="C8">
+        <v>13.523</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>94.039490667500004</v>
+        <v>94.155000000000001</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G8" s="5">
-        <v>277.78013015300002</v>
+        <v>280.14100000000002</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="5">
-        <v>357.18574971999999</v>
+      <c r="I8">
+        <v>362.99</v>
       </c>
       <c r="J8" t="s">
         <v>40</v>
@@ -5863,28 +6003,28 @@
       </c>
       <c r="C9" s="5">
         <f>(C8)/C7</f>
-        <v>1.075942232339373</v>
+        <v>1.2701230393538088</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="5">
         <f>(E8)/E7</f>
-        <v>1.1036208336654731</v>
+        <v>1.0913358446827008</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="5">
         <f>(G8)/G7</f>
-        <v>1.1167179495051449</v>
+        <v>1.1452744413464919</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I9" s="5">
         <f>(I8)/I7</f>
-        <v>0.98603960581602212</v>
+        <v>1.0026461749237636</v>
       </c>
       <c r="J9" t="s">
         <v>40</v>
@@ -5968,26 +6108,26 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.614573017</v>
+      <c r="C15" s="5">
+        <v>0.64300000000000002</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="2">
-        <v>2.0768330289999999</v>
+      <c r="E15" s="5">
+        <v>1.9330000000000001</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="2">
-        <v>5.3738602850000001</v>
+      <c r="G15" s="5">
+        <v>4.4969999999999999</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I15" s="2">
-        <v>7.7896056939999996</v>
+      <c r="I15" s="5">
+        <v>6.3239999999999998</v>
       </c>
       <c r="J15" t="s">
         <v>40</v>
@@ -6000,26 +6140,26 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="2">
-        <v>4.9632009999999997E-2</v>
+      <c r="C16" s="5">
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="2">
-        <v>1.416479233</v>
+      <c r="E16" s="5">
+        <v>1.45</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="2">
-        <v>9.3476763569999992</v>
+      <c r="G16" s="5">
+        <v>9.3089999999999993</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I16" s="2">
-        <v>12</v>
+      <c r="I16" s="5">
+        <v>11.96</v>
       </c>
       <c r="J16" t="s">
         <v>40</v>
@@ -6032,26 +6172,26 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2">
-        <v>0.19636084000000001</v>
+      <c r="C17" s="5">
+        <v>0.18099999999999999</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="2">
-        <v>2.4097560869999999</v>
+      <c r="E17" s="5">
+        <v>2.5760000000000001</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="2">
-        <v>12.41054997</v>
+      <c r="G17" s="5">
+        <v>12.532</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I17" s="2">
-        <v>19.448379490000001</v>
+      <c r="I17" s="5">
+        <v>19.335000000000001</v>
       </c>
       <c r="J17" t="s">
         <v>40</v>
@@ -6064,26 +6204,26 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="2">
-        <v>4.0852307999999997E-2</v>
+      <c r="C18" s="5">
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="2">
-        <v>0.14858833499999999</v>
+      <c r="E18" s="5">
+        <v>0.251</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="2">
-        <v>7.8177788110000002</v>
+      <c r="G18" s="5">
+        <v>8.5370000000000008</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="2">
-        <v>12.330035049999999</v>
+      <c r="I18" s="5">
+        <v>12.845000000000001</v>
       </c>
       <c r="J18" t="s">
         <v>40</v>
@@ -6096,26 +6236,26 @@
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="2">
-        <v>0.20614339700000001</v>
+      <c r="C19" s="5">
+        <v>0.186</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="2">
-        <v>1.6606400859999999</v>
+      <c r="E19" s="5">
+        <v>1.03</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="2">
-        <v>6.1319755020000004</v>
+      <c r="G19" s="5">
+        <v>2.9689999999999999</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I19" s="2">
-        <v>10.311542640000001</v>
+      <c r="I19" s="5">
+        <v>5.6449999999999996</v>
       </c>
       <c r="J19" t="s">
         <v>40</v>
@@ -6142,28 +6282,28 @@
       </c>
       <c r="C21" s="5">
         <f>SUM(C15:C19)</f>
-        <v>1.1075615719999998</v>
+        <v>1.1279999999999999</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="5">
         <f>SUM(E15:E19)</f>
-        <v>7.71229677</v>
+        <v>7.24</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G21" s="5">
         <f>SUM(G15:G19)</f>
-        <v>41.081840925000009</v>
+        <v>37.844000000000001</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I21" s="5">
         <f>SUM(I15:I19)</f>
-        <v>61.879562873999994</v>
+        <v>56.108999999999995</v>
       </c>
       <c r="J21" t="s">
         <v>40</v>
@@ -6176,26 +6316,26 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2">
-        <v>1.6511213220000001</v>
+      <c r="C22" s="5">
+        <v>1.7849999999999999</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="2">
-        <v>7.0253575079999999</v>
+      <c r="E22" s="5">
+        <v>7.0650000000000004</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G22" s="2">
-        <v>37.873027069999999</v>
+      <c r="G22" s="5">
+        <v>37.359000000000002</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I22" s="2">
-        <v>49.35974126</v>
+      <c r="I22" s="5">
+        <v>49.334000000000003</v>
       </c>
       <c r="J22" t="s">
         <v>40</v>
@@ -6210,28 +6350,28 @@
       </c>
       <c r="C23" s="5">
         <f t="shared" ref="C23:H23" si="1">(C22)/C21</f>
-        <v>1.4907715866472842</v>
+        <v>1.5824468085106385</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" si="1"/>
-        <v>0.91092935315039747</v>
+        <v>0.975828729281768</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="1"/>
-        <v>0.92189216006999064</v>
+        <v>0.98718422999682909</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="5">
         <f>(I22)/I21</f>
-        <v>0.79767436884625342</v>
+        <v>0.87925288278172853</v>
       </c>
       <c r="J23" t="s">
         <v>40</v>
@@ -6306,40 +6446,40 @@
       <c r="B27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="2">
-        <v>9.7880270849999995</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27">
+      <c r="C27" s="5">
+        <v>10.282999999999999</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
         <v>9.6999999999999993</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2">
-        <v>101.7042635</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>449.60469970000003</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="F27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>101.48699999999999</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="5">
+        <v>419.411</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K27" s="2">
         <v>401</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M27" s="2">
-        <v>639.16812279999999</v>
-      </c>
-      <c r="N27" s="1" t="s">
+      <c r="L27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <v>525.90099999999995</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O27" s="2">
@@ -6356,40 +6496,40 @@
       <c r="B28" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="2">
-        <v>3.6177842120000001</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28">
+      <c r="C28" s="5">
+        <v>3.7970000000000002</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
         <v>4</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2">
-        <v>91.090846869999993</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2">
-        <v>357.63365320000003</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="F28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>88.95</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5">
+        <v>337.22300000000001</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K28" s="2">
         <v>368</v>
       </c>
-      <c r="L28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M28" s="2">
-        <v>367.35382920000001</v>
-      </c>
-      <c r="N28" s="1" t="s">
+      <c r="L28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="5">
+        <v>352.065</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O28" s="2">
@@ -6406,40 +6546,40 @@
       <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="2">
-        <v>110.0219116</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29">
+      <c r="C29" s="5">
+        <v>110.56699999999999</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
         <v>110</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
-        <v>812.83911339999997</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1857.3335959999999</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="F29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>830.96699999999998</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="5">
+        <v>2065.1260000000002</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K29" s="2">
         <v>1585</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M29" s="2">
-        <v>2000.9436270000001</v>
-      </c>
-      <c r="N29" s="1" t="s">
+      <c r="L29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="5">
+        <v>2278.6129999999998</v>
+      </c>
+      <c r="N29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O29" s="2">
@@ -6460,6 +6600,12 @@
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
@@ -6470,47 +6616,47 @@
       </c>
       <c r="C31" s="2">
         <f>SUM(C27:C29)</f>
-        <v>123.427722897</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31">
+        <v>124.64699999999999</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
         <f>SUM(E27:E29)</f>
         <v>123.7</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G31" s="2">
         <f>SUM(G27:G29)</f>
-        <v>1005.6342237699999</v>
-      </c>
-      <c r="H31" s="1" t="s">
+        <v>1021.404</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" ref="I31" si="2">SUM(I27:I29)</f>
-        <v>2664.5719489000003</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31">
+        <v>2821.76</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="5">
         <f>SUM(K27:K29)</f>
         <v>2354</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="L31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M31" s="2">
         <f t="shared" ref="M31" si="3">SUM(M27:M29)</f>
-        <v>3007.4655790000002</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O31">
+        <v>3156.5789999999997</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5">
         <f>SUM(O27:O29)</f>
         <v>3330</v>
       </c>
@@ -6525,40 +6671,40 @@
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="2">
-        <v>135.26027999999999</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32">
+      <c r="C32" s="5">
+        <v>135.19800000000001</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5">
         <v>145</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1195.2043180000001</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2">
-        <v>4450.3103659999997</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="F32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1194.568</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="5">
+        <v>4449.4579999999996</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="2">
         <v>3780</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M32" s="2">
-        <v>5910.258425</v>
-      </c>
-      <c r="N32" s="1" t="s">
+      <c r="L32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M32" s="5">
+        <v>5840.6390000000001</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O32" s="2">
@@ -6577,44 +6723,44 @@
       </c>
       <c r="C33" s="5">
         <f>(C32)/C31</f>
-        <v>1.0958662837268272</v>
-      </c>
-      <c r="D33" s="1" t="s">
+        <v>1.0846470432501385</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E33" s="5">
         <f>(E32)/E31</f>
         <v>1.1721907841552142</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="5">
         <f>(G32)/G31</f>
-        <v>1.1885079979869071</v>
-      </c>
-      <c r="H33" s="1" t="s">
+        <v>1.1695352671420907</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I33" s="5">
         <f>(I32)/I31</f>
-        <v>1.6701783443442746</v>
-      </c>
-      <c r="J33" s="1" t="s">
+        <v>1.5768378600589701</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K33" s="5">
         <f>(K32)/K31</f>
         <v>1.6057774001699234</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="L33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M33" s="5">
         <f>(M32)/M31</f>
-        <v>1.9651957004160279</v>
-      </c>
-      <c r="N33" s="1" t="s">
+        <v>1.8503066135838833</v>
+      </c>
+      <c r="N33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O33" s="5">
@@ -6644,7 +6790,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7756,7 +7902,7 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="8" t="s">
         <v>185</v>
       </c>
       <c r="B44" t="s">
@@ -7793,7 +7939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D11"/>
     </sheetView>
   </sheetViews>
@@ -7923,4 +8069,1213 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN21"/>
+  <sheetViews>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AK10" sqref="AK10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:40">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" t="s">
+        <v>118</v>
+      </c>
+      <c r="X1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.214</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2.1395888924599999E-2</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="1">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O3">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>4.4969999999999999</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>6.3239999999999998</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2E-3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4">
+        <v>1.4E-2</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S4">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0.308</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>5.5E-2</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="AD4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>0.191</v>
+      </c>
+      <c r="AF4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>9.3089999999999993</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>11.96</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>1.1930000000000001</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="6">
+        <v>2.7946682646900001E-3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0.09</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0.218</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>2.5760000000000001</v>
+      </c>
+      <c r="AD5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="AF5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>12.532</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>0.94</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>19.335000000000001</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>1.4119999999999999</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2E-3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>5.5E-2</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>0.251</v>
+      </c>
+      <c r="AD6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>8.5370000000000008</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>12.845000000000001</v>
+      </c>
+      <c r="AL6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>1.252</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4.2455147951799997E-3</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S7">
+        <v>2.4E-2</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>0.32</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W7">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>0.186</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>1.03</v>
+      </c>
+      <c r="AD7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="AF7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>2.9689999999999999</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>5.6449999999999996</v>
+      </c>
+      <c r="AL7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0.155</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.55428335071E-2</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1.113</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S8">
+        <v>0.111</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1.8049999999999999</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W8">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>1.8089999999999999</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>2.2919999999999998</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>1.6359999999999999</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>1.216</v>
+      </c>
+      <c r="AL8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM8" s="5">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
+      <c r="A9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2E-3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O9">
+        <v>2E-3</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>0.06</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S9">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W9">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>0.111</v>
+      </c>
+      <c r="AD9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AF9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="AH9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AJ9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>2.0880000000000001</v>
+      </c>
+      <c r="AL9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM9" s="5">
+        <v>0.312</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
+      <c r="I10">
+        <v>0.108</v>
+      </c>
+      <c r="K10" s="1">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="M10">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="O10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Q10">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="S10">
+        <v>2.4E-2</v>
+      </c>
+      <c r="U10">
+        <v>0.315</v>
+      </c>
+      <c r="W10">
+        <v>3.1E-2</v>
+      </c>
+      <c r="Y10">
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>7.0650000000000004</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>0.51</v>
+      </c>
+      <c r="AG10">
+        <v>37.359000000000002</v>
+      </c>
+      <c r="AI10">
+        <v>2.6179999999999999</v>
+      </c>
+      <c r="AK10">
+        <v>49.334000000000003</v>
+      </c>
+      <c r="AM10">
+        <v>3.456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
+      <c r="AC11" s="5"/>
+    </row>
+    <row r="14" spans="1:40">
+      <c r="I14">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="J14">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K14">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="M14">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="N14">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="O14">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="P14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40">
+      <c r="I15">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="J15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K15">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="L15">
+        <v>1.4E-2</v>
+      </c>
+      <c r="M15">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="N15">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="O15">
+        <v>0.308</v>
+      </c>
+      <c r="P15">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40">
+      <c r="I16">
+        <v>0.09</v>
+      </c>
+      <c r="J16">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K16">
+        <v>0.218</v>
+      </c>
+      <c r="L16">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="N16">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="O16">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="P16">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="9:16">
+      <c r="I17">
+        <v>2.3E-2</v>
+      </c>
+      <c r="J17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="L17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="N17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O17">
+        <v>5.5E-2</v>
+      </c>
+      <c r="P17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="9:16">
+      <c r="I18">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J18">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="L18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M18">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="N18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="O18">
+        <v>0.32</v>
+      </c>
+      <c r="P18">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="9:16">
+      <c r="I19">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="J19">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K19">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="L19">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M19">
+        <v>1.113</v>
+      </c>
+      <c r="N19">
+        <v>0.111</v>
+      </c>
+      <c r="O19">
+        <v>1.8049999999999999</v>
+      </c>
+      <c r="P19">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="9:16">
+      <c r="I20">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J20">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K20">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L20">
+        <v>2E-3</v>
+      </c>
+      <c r="M20">
+        <v>0.06</v>
+      </c>
+      <c r="N20">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O20">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="P20">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="9:16">
+      <c r="I21">
+        <v>0.108</v>
+      </c>
+      <c r="J21">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K21">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L21">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="M21">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="N21">
+        <v>2.4E-2</v>
+      </c>
+      <c r="O21">
+        <v>0.315</v>
+      </c>
+      <c r="P21">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a bunch of pictures
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="223">
   <si>
     <t>\toprule</t>
   </si>
@@ -692,6 +692,9 @@
   </si>
   <si>
     <t>20h07m07.927s +27d27m15.782s</t>
+  </si>
+  <si>
+    <t>Jy</t>
   </si>
 </sst>
 </file>
@@ -750,8 +753,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="369">
+  <cellStyleXfs count="393">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1134,7 +1161,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="369">
+  <cellStyles count="393">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1319,6 +1346,18 @@
     <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1503,6 +1542,18 @@
     <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5756,10 +5807,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection sqref="A1:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5814,69 +5865,67 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>42</v>
+      <c r="A2" s="1"/>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>10.071999999999999</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>72.040999999999997</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>167.929</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5">
-        <v>234.93</v>
-      </c>
-      <c r="J3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5">
-        <v>0.38300000000000001</v>
+        <v>10.071999999999999</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>11.207000000000001</v>
+        <v>72.040999999999997</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>56.703000000000003</v>
+        <v>167.929</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>89.546000000000006</v>
+        <v>234.93</v>
       </c>
       <c r="J4" t="s">
         <v>40</v>
@@ -5884,31 +5933,31 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0.192</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>3.0270000000000001</v>
+        <v>11.207000000000001</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="5">
-        <v>19.974</v>
+        <v>56.703000000000003</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>37.555999999999997</v>
+        <v>89.546000000000006</v>
       </c>
       <c r="J5" t="s">
         <v>40</v>
@@ -5916,128 +5965,151 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.192</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3.0270000000000001</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
+        <v>19.974</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="5">
+        <v>37.555999999999997</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>110</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <f>SUM(C3:C5)</f>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <f>SUM(C4:C6)</f>
         <v>10.646999999999998</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <f t="shared" ref="E7:I7" si="0">SUM(E3:E5)</f>
+      <c r="D8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:I8" si="0">SUM(E4:E6)</f>
         <v>86.274999999999991</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>244.60599999999999</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="H8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
         <f t="shared" si="0"/>
         <v>362.03199999999998</v>
       </c>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="1" t="s">
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
         <v>13.523</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="D9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>94.155000000000001</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
         <v>280.14100000000002</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8">
+      <c r="H9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>362.99</v>
       </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>200</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <f>(C8)/C7</f>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <f>(C9)/C8</f>
         <v>1.2701230393538088</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <f>(E8)/E7</f>
+      <c r="D10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <f>(E9)/E8</f>
         <v>1.0913358446827008</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="5">
-        <f>(G8)/G7</f>
+      <c r="F10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <f>(G9)/G8</f>
         <v>1.1452744413464919</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="5">
-        <f>(I8)/I7</f>
+      <c r="H10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <f>(I9)/I8</f>
         <v>1.0026461749237636</v>
       </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="5"/>
@@ -6058,140 +6130,115 @@
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="1" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
+      <c r="F14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="H14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>222</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>222</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1.9330000000000001</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>4.4969999999999999</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="5">
-        <v>6.3239999999999998</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1.45</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="5">
-        <v>9.3089999999999993</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="5">
-        <v>11.96</v>
-      </c>
-      <c r="J16" t="s">
-        <v>40</v>
-      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>0.18099999999999999</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="5">
-        <v>2.5760000000000001</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="5">
-        <v>12.532</v>
+        <v>4.4969999999999999</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I17" s="5">
-        <v>19.335000000000001</v>
+        <v>6.3239999999999998</v>
       </c>
       <c r="J17" t="s">
         <v>40</v>
@@ -6199,7 +6246,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -6211,19 +6258,19 @@
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <v>0.251</v>
+        <v>1.45</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G18" s="5">
-        <v>8.5370000000000008</v>
+        <v>9.3089999999999993</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I18" s="5">
-        <v>12.845000000000001</v>
+        <v>11.96</v>
       </c>
       <c r="J18" t="s">
         <v>40</v>
@@ -6231,434 +6278,414 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2.5760000000000001</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>12.532</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>19.335000000000001</v>
+      </c>
+      <c r="J19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.251</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>8.5370000000000008</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="5">
+        <v>12.845000000000001</v>
+      </c>
+      <c r="J20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
         <v>0.186</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="D21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
         <v>1.03</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="F21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
         <v>2.9689999999999999</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5">
+      <c r="H21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
         <v>5.6449999999999996</v>
       </c>
-      <c r="J19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
-      <c r="A20" t="s">
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:16">
-      <c r="A21" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <f>SUM(C15:C19)</f>
-        <v>1.1279999999999999</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5">
-        <f>SUM(E15:E19)</f>
-        <v>7.24</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="5">
-        <f>SUM(G15:G19)</f>
-        <v>37.844000000000001</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5">
-        <f>SUM(I15:I19)</f>
-        <v>56.108999999999995</v>
-      </c>
-      <c r="J21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
-        <v>1.7849999999999999</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5">
-        <v>7.0650000000000004</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="5">
-        <v>37.359000000000002</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="5">
-        <v>49.334000000000003</v>
-      </c>
-      <c r="J22" t="s">
-        <v>40</v>
-      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <f>SUM(C17:C21)</f>
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <f>SUM(E17:E21)</f>
+        <v>7.24</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="5">
+        <f>SUM(G17:G21)</f>
+        <v>37.844000000000001</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="5">
+        <f>SUM(I17:I21)</f>
+        <v>56.108999999999995</v>
+      </c>
+      <c r="J23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1.7849999999999999</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="5">
+        <v>7.0650000000000004</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>37.359000000000002</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="5">
+        <v>49.334000000000003</v>
+      </c>
+      <c r="J24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
         <v>200</v>
       </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5">
-        <f t="shared" ref="C23:H23" si="1">(C22)/C21</f>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" ref="C25:H25" si="1">(C24)/C23</f>
         <v>1.5824468085106385</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5">
+      <c r="D25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
         <f t="shared" si="1"/>
         <v>0.975828729281768</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="5">
+      <c r="F25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="5">
         <f t="shared" si="1"/>
         <v>0.98718422999682909</v>
       </c>
-      <c r="H23" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="5">
-        <f>(I22)/I21</f>
+      <c r="H25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="5">
+        <f>(I24)/I23</f>
         <v>0.87925288278172853</v>
       </c>
-      <c r="J23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="P25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="J25" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>222</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>222</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>222</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>222</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>222</v>
+      </c>
+      <c r="P28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="5">
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
         <v>10.282999999999999</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="5">
+      <c r="D30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
         <v>9.6999999999999993</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="5">
         <v>101.48699999999999</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" s="5">
+      <c r="H30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="5">
         <v>419.411</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K27" s="2">
+      <c r="J30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" s="2">
         <v>401</v>
       </c>
-      <c r="L27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M27" s="5">
+      <c r="L30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M30" s="5">
         <v>525.90099999999995</v>
       </c>
-      <c r="N27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O27" s="2">
+      <c r="N30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2">
         <v>669</v>
       </c>
-      <c r="P27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="1" t="s">
+      <c r="P30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="5">
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
         <v>3.7970000000000002</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="D31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5">
         <v>4</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="5">
+      <c r="F31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="5">
         <v>88.95</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="5">
+      <c r="H31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
         <v>337.22300000000001</v>
       </c>
-      <c r="J28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K28" s="2">
+      <c r="J31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2">
         <v>368</v>
       </c>
-      <c r="L28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M28" s="5">
+      <c r="L31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M31" s="5">
         <v>352.065</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O28" s="2">
+      <c r="N31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" s="2">
         <v>485</v>
-      </c>
-      <c r="P28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5">
-        <v>110.56699999999999</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="5">
-        <v>110</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="5">
-        <v>830.96699999999998</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="5">
-        <v>2065.1260000000002</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1585</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M29" s="5">
-        <v>2278.6129999999998</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O29" s="2">
-        <v>2176</v>
-      </c>
-      <c r="P29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:16">
-      <c r="A31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <f>SUM(C27:C29)</f>
-        <v>124.64699999999999</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5">
-        <f>SUM(E27:E29)</f>
-        <v>123.7</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <f>SUM(G27:G29)</f>
-        <v>1021.404</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2">
-        <f t="shared" ref="I31" si="2">SUM(I27:I29)</f>
-        <v>2821.76</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K31" s="5">
-        <f>SUM(K27:K29)</f>
-        <v>2354</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <f t="shared" ref="M31" si="3">SUM(M27:M29)</f>
-        <v>3156.5789999999997</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O31" s="5">
-        <f>SUM(O27:O29)</f>
-        <v>3330</v>
       </c>
       <c r="P31" t="s">
         <v>40</v>
@@ -6666,49 +6693,49 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C32" s="5">
-        <v>135.19800000000001</v>
+        <v>110.56699999999999</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E32" s="5">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G32" s="5">
-        <v>1194.568</v>
+        <v>830.96699999999998</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I32" s="5">
-        <v>4449.4579999999996</v>
+        <v>2065.1260000000002</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K32" s="2">
-        <v>3780</v>
+        <v>1585</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M32" s="5">
-        <v>5840.6390000000001</v>
+        <v>2278.6129999999998</v>
       </c>
       <c r="N32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O32" s="2">
-        <v>6730</v>
+        <v>2176</v>
       </c>
       <c r="P32" t="s">
         <v>40</v>
@@ -6716,63 +6743,188 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2">
+        <f>SUM(C30:C32)</f>
+        <v>124.64699999999999</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5">
+        <f>SUM(E30:E32)</f>
+        <v>123.7</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <f>SUM(G30:G32)</f>
+        <v>1021.404</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" ref="I34" si="2">SUM(I30:I32)</f>
+        <v>2821.76</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" s="5">
+        <f>SUM(K30:K32)</f>
+        <v>2354</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" ref="M34" si="3">SUM(M30:M32)</f>
+        <v>3156.5789999999997</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34" s="5">
+        <f>SUM(O30:O32)</f>
+        <v>3330</v>
+      </c>
+      <c r="P34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5">
+        <v>135.19800000000001</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5">
+        <v>145</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1194.568</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5">
+        <v>4449.4579999999996</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" s="2">
+        <v>3780</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="5">
+        <v>5840.6390000000001</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" s="2">
+        <v>6730</v>
+      </c>
+      <c r="P35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
         <v>200</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5">
-        <f>(C32)/C31</f>
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5">
+        <f>(C35)/C34</f>
         <v>1.0846470432501385</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5">
-        <f>(E32)/E31</f>
+      <c r="D36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5">
+        <f>(E35)/E34</f>
         <v>1.1721907841552142</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G33" s="5">
-        <f>(G32)/G31</f>
+      <c r="F36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <f>(G35)/G34</f>
         <v>1.1695352671420907</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I33" s="5">
-        <f>(I32)/I31</f>
+      <c r="H36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
+        <f>(I35)/I34</f>
         <v>1.5768378600589701</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K33" s="5">
-        <f>(K32)/K31</f>
+      <c r="J36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" s="5">
+        <f>(K35)/K34</f>
         <v>1.6057774001699234</v>
       </c>
-      <c r="L33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M33" s="5">
-        <f>(M32)/M31</f>
+      <c r="L36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" s="5">
+        <f>(M35)/M34</f>
         <v>1.8503066135838833</v>
       </c>
-      <c r="N33" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O33" s="5">
-        <f>(O32)/O31</f>
+      <c r="N36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O36" s="5">
+        <f>(O35)/O34</f>
         <v>2.0210210210210211</v>
       </c>
-      <c r="P33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="1"/>
+      <c r="P36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8073,10 +8225,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN21"/>
+  <dimension ref="A1:AN22"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AK10" sqref="AK10"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8150,249 +8302,189 @@
       </c>
     </row>
     <row r="2" spans="1:40">
-      <c r="A2" t="s">
-        <v>42</v>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>222</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>222</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>222</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:40">
       <c r="A3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.214</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G3" s="6">
-        <v>2.1395888924599999E-2</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.48899999999999999</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="O3">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="S3">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="W3">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>1.9330000000000001</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>0.20200000000000001</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>4.4969999999999999</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="5">
-        <v>6.3239999999999998</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="AM3" s="5">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:40">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>2E-3</v>
+        <v>0.214</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="6">
-        <v>1.5E-3</v>
+        <v>2.1395888924599999E-2</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>4.1000000000000002E-2</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K4" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M4">
-        <v>0.14199999999999999</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O4">
-        <v>1.4E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="P4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q4">
-        <v>0.26400000000000001</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="R4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S4">
-        <v>2.5999999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U4">
-        <v>0.308</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W4">
-        <v>3.1E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y4" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>0.64300000000000002</v>
       </c>
       <c r="Z4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA4" s="5">
-        <v>5.5E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="AB4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC4" s="5">
-        <v>1.45</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE4" s="5">
-        <v>0.191</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="AF4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG4" s="5">
-        <v>9.3089999999999993</v>
+        <v>4.4969999999999999</v>
       </c>
       <c r="AH4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI4" s="5">
-        <v>0.71599999999999997</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="AJ4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK4" s="5">
-        <v>11.96</v>
+        <v>6.3239999999999998</v>
       </c>
       <c r="AL4" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM4" s="5">
-        <v>1.1930000000000001</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="AN4" t="s">
         <v>40</v>
@@ -8400,121 +8492,121 @@
     </row>
     <row r="5" spans="1:40">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>2.8000000000000001E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G5" s="6">
-        <v>2.7946682646900001E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0.09</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K5" s="1">
-        <v>8.9999999999999993E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M5">
-        <v>0.218</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="N5" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O5">
-        <v>2.1999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q5">
-        <v>0.33900000000000002</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S5">
-        <v>3.4000000000000002E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U5">
-        <v>0.42899999999999999</v>
+        <v>0.308</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W5">
-        <v>4.2999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="X5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y5" s="5">
-        <v>0.18099999999999999</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="Z5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA5" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AB5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC5" s="5">
-        <v>2.5760000000000001</v>
+        <v>1.45</v>
       </c>
       <c r="AD5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE5" s="5">
-        <v>0.26600000000000001</v>
+        <v>0.191</v>
       </c>
       <c r="AF5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG5" s="5">
-        <v>12.532</v>
+        <v>9.3089999999999993</v>
       </c>
       <c r="AH5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI5" s="5">
-        <v>0.94</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="AJ5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK5" s="5">
-        <v>19.335000000000001</v>
+        <v>11.96</v>
       </c>
       <c r="AL5" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM5" s="5">
-        <v>1.4119999999999999</v>
+        <v>1.1930000000000001</v>
       </c>
       <c r="AN5" t="s">
         <v>40</v>
@@ -8522,121 +8614,121 @@
     </row>
     <row r="6" spans="1:40">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>2E-3</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G6" s="6">
-        <v>1.5E-3</v>
+        <v>2.7946682646900001E-3</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>2.3E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K6" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="L6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M6">
-        <v>3.9E-2</v>
+        <v>0.218</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O6">
-        <v>4.0000000000000001E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>5.2999999999999999E-2</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S6">
-        <v>8.0000000000000002E-3</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U6">
-        <v>5.5E-2</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W6">
-        <v>8.0000000000000002E-3</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="X6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y6" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="Z6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA6" s="5">
-        <v>5.2999999999999999E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AB6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC6" s="5">
-        <v>0.251</v>
+        <v>2.5760000000000001</v>
       </c>
       <c r="AD6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE6" s="5">
-        <v>0.19600000000000001</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="AF6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG6" s="5">
-        <v>8.5370000000000008</v>
+        <v>12.532</v>
       </c>
       <c r="AH6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI6" s="5">
-        <v>0.79500000000000004</v>
+        <v>0.94</v>
       </c>
       <c r="AJ6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK6" s="5">
-        <v>12.845000000000001</v>
+        <v>19.335000000000001</v>
       </c>
       <c r="AL6" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM6" s="5">
-        <v>1.252</v>
+        <v>1.4119999999999999</v>
       </c>
       <c r="AN6" t="s">
         <v>40</v>
@@ -8644,121 +8736,121 @@
     </row>
     <row r="7" spans="1:40">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>4.2000000000000003E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G7" s="6">
-        <v>4.2455147951799997E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>0.11799999999999999</v>
+        <v>2.3E-2</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K7" s="1">
-        <v>1.2E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M7">
-        <v>0.17599999999999999</v>
+        <v>3.9E-2</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O7">
-        <v>1.7999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>0.23499999999999999</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S7">
-        <v>2.4E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U7">
-        <v>0.32</v>
+        <v>5.5E-2</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W7">
-        <v>3.2000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="X7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y7" s="5">
-        <v>0.186</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="Z7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA7" s="5">
-        <v>5.1999999999999998E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AB7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC7" s="5">
-        <v>1.03</v>
+        <v>0.251</v>
       </c>
       <c r="AD7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE7" s="5">
-        <v>0.21199999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="AF7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG7" s="5">
-        <v>2.9689999999999999</v>
+        <v>8.5370000000000008</v>
       </c>
       <c r="AH7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI7" s="5">
-        <v>0.32600000000000001</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="AJ7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK7" s="5">
-        <v>5.6449999999999996</v>
+        <v>12.845000000000001</v>
       </c>
       <c r="AL7" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM7" s="5">
-        <v>0.65200000000000002</v>
+        <v>1.252</v>
       </c>
       <c r="AN7" t="s">
         <v>40</v>
@@ -8766,121 +8858,121 @@
     </row>
     <row r="8" spans="1:40">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0.155</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="6">
-        <v>1.55428335071E-2</v>
+        <v>4.2455147951799997E-3</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.53700000000000003</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K8" s="1">
-        <v>5.3999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M8">
-        <v>0.77100000000000002</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="N8" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O8">
-        <v>7.6999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q8">
-        <v>1.113</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="R8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S8">
-        <v>0.111</v>
+        <v>2.4E-2</v>
       </c>
       <c r="T8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U8">
-        <v>1.8049999999999999</v>
+        <v>0.32</v>
       </c>
       <c r="V8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W8">
-        <v>0.18099999999999999</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="X8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y8" s="5">
-        <v>1.8089999999999999</v>
+        <v>0.186</v>
       </c>
       <c r="Z8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA8" s="5">
-        <v>0.13300000000000001</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="AB8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC8" s="5">
-        <v>2.2919999999999998</v>
+        <v>1.03</v>
       </c>
       <c r="AD8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE8" s="5">
-        <v>0.16900000000000001</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="AF8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG8" s="5">
-        <v>1.6359999999999999</v>
+        <v>2.9689999999999999</v>
       </c>
       <c r="AH8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI8" s="5">
-        <v>0.13700000000000001</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="AJ8" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK8" s="5">
-        <v>1.216</v>
+        <v>5.6449999999999996</v>
       </c>
       <c r="AL8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM8" s="5">
-        <v>0.38100000000000001</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="AN8" t="s">
         <v>40</v>
@@ -8888,384 +8980,506 @@
     </row>
     <row r="9" spans="1:40">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>2E-3</v>
+        <v>0.155</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="G9" s="6">
-        <v>1.5E-3</v>
+        <v>1.55428335071E-2</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>4.0000000000000001E-3</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="K9" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="M9">
-        <v>2.4E-2</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="N9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="O9">
-        <v>2E-3</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Q9">
-        <v>0.06</v>
+        <v>1.113</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="S9">
-        <v>6.0000000000000001E-3</v>
+        <v>0.111</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="U9">
-        <v>7.1999999999999995E-2</v>
+        <v>1.8049999999999999</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="W9">
-        <v>7.0000000000000001E-3</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="X9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="Y9" s="5">
-        <v>5.8999999999999997E-2</v>
+        <v>1.8089999999999999</v>
       </c>
       <c r="Z9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AA9" s="5">
-        <v>5.2999999999999999E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="AB9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AC9" s="5">
-        <v>0.111</v>
+        <v>2.2919999999999998</v>
       </c>
       <c r="AD9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AE9" s="5">
-        <v>5.8000000000000003E-2</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="AF9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AG9" s="5">
-        <v>1.1459999999999999</v>
+        <v>1.6359999999999999</v>
       </c>
       <c r="AH9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AI9" s="5">
-        <v>0.14299999999999999</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="AJ9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AK9" s="5">
-        <v>2.0880000000000001</v>
+        <v>1.216</v>
       </c>
       <c r="AL9" s="5" t="s">
         <v>82</v>
       </c>
       <c r="AM9" s="5">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
+      <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2E-3</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>2.4E-2</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O10">
+        <v>2E-3</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>0.06</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="S10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="W10">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>0.111</v>
+      </c>
+      <c r="AD10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="AH10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="AJ10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>2.0880000000000001</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM10" s="5">
         <v>0.312</v>
       </c>
-      <c r="AN9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40">
-      <c r="I10">
+      <c r="AN10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40">
+      <c r="I11">
         <v>0.108</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K11" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="M10">
+      <c r="M11">
         <v>0.17299999999999999</v>
       </c>
-      <c r="O10">
+      <c r="O11">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="Q10">
+      <c r="Q11">
         <v>0.24099999999999999</v>
       </c>
-      <c r="S10">
+      <c r="S11">
         <v>2.4E-2</v>
       </c>
-      <c r="U10">
+      <c r="U11">
         <v>0.315</v>
       </c>
-      <c r="W10">
+      <c r="W11">
         <v>3.1E-2</v>
       </c>
-      <c r="Y10">
+      <c r="Y11">
         <v>1.7849999999999999</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AA11" s="5">
         <v>0.13</v>
       </c>
-      <c r="AC10" s="5">
+      <c r="AC11" s="5">
         <v>7.0650000000000004</v>
       </c>
-      <c r="AE10" s="5">
+      <c r="AE11" s="5">
         <v>0.51</v>
       </c>
-      <c r="AG10">
+      <c r="AG11">
         <v>37.359000000000002</v>
       </c>
-      <c r="AI10">
+      <c r="AI11">
         <v>2.6179999999999999</v>
       </c>
-      <c r="AK10">
+      <c r="AK11">
         <v>49.334000000000003</v>
       </c>
-      <c r="AM10">
+      <c r="AM11">
         <v>3.456</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
-      <c r="AC11" s="5"/>
-    </row>
-    <row r="14" spans="1:40">
-      <c r="I14">
-        <v>0.48899999999999999</v>
-      </c>
-      <c r="J14">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="K14">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="L14">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="M14">
-        <v>0.73099999999999998</v>
-      </c>
-      <c r="N14">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="O14">
-        <v>0.85799999999999998</v>
-      </c>
-      <c r="P14">
-        <v>8.5999999999999993E-2</v>
-      </c>
+    <row r="12" spans="1:40">
+      <c r="AC12" s="5"/>
     </row>
     <row r="15" spans="1:40">
       <c r="I15">
-        <v>4.1000000000000002E-2</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="J15">
-        <v>4.0000000000000001E-3</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="K15">
-        <v>0.14199999999999999</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="L15">
-        <v>1.4E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="M15">
-        <v>0.26400000000000001</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="N15">
-        <v>2.5999999999999999E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="O15">
-        <v>0.308</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="P15">
-        <v>3.1E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="16" spans="1:40">
       <c r="I16">
-        <v>0.09</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="J16">
-        <v>8.9999999999999993E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="K16">
-        <v>0.218</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="L16">
-        <v>2.1999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="M16">
-        <v>0.33900000000000002</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="N16">
-        <v>3.4000000000000002E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="O16">
-        <v>0.42899999999999999</v>
+        <v>0.308</v>
       </c>
       <c r="P16">
-        <v>4.2999999999999997E-2</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="17" spans="9:16">
       <c r="I17">
-        <v>2.3E-2</v>
+        <v>0.09</v>
       </c>
       <c r="J17">
-        <v>3.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="K17">
-        <v>3.9E-2</v>
+        <v>0.218</v>
       </c>
       <c r="L17">
-        <v>4.0000000000000001E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M17">
-        <v>5.2999999999999999E-2</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="N17">
-        <v>8.0000000000000002E-3</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="O17">
-        <v>5.5E-2</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="P17">
-        <v>8.0000000000000002E-3</v>
+        <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="9:16">
       <c r="I18">
-        <v>0.11799999999999999</v>
+        <v>2.3E-2</v>
       </c>
       <c r="J18">
-        <v>1.2E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="K18">
-        <v>0.17599999999999999</v>
+        <v>3.9E-2</v>
       </c>
       <c r="L18">
-        <v>1.7999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M18">
-        <v>0.23499999999999999</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="N18">
-        <v>2.4E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="O18">
-        <v>0.32</v>
+        <v>5.5E-2</v>
       </c>
       <c r="P18">
-        <v>3.2000000000000001E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="19" spans="9:16">
       <c r="I19">
-        <v>0.53700000000000003</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="J19">
-        <v>5.3999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K19">
-        <v>0.77100000000000002</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="L19">
-        <v>7.6999999999999999E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M19">
-        <v>1.113</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="N19">
-        <v>0.111</v>
+        <v>2.4E-2</v>
       </c>
       <c r="O19">
-        <v>1.8049999999999999</v>
+        <v>0.32</v>
       </c>
       <c r="P19">
-        <v>0.18099999999999999</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="9:16">
       <c r="I20">
-        <v>4.0000000000000001E-3</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="J20">
-        <v>4.0000000000000001E-3</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="K20">
-        <v>2.4E-2</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="L20">
-        <v>2E-3</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="M20">
-        <v>0.06</v>
+        <v>1.113</v>
       </c>
       <c r="N20">
-        <v>6.0000000000000001E-3</v>
+        <v>0.111</v>
       </c>
       <c r="O20">
-        <v>7.1999999999999995E-2</v>
+        <v>1.8049999999999999</v>
       </c>
       <c r="P20">
-        <v>7.0000000000000001E-3</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="21" spans="9:16">
       <c r="I21">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J21">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K21">
+        <v>2.4E-2</v>
+      </c>
+      <c r="L21">
+        <v>2E-3</v>
+      </c>
+      <c r="M21">
+        <v>0.06</v>
+      </c>
+      <c r="N21">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O21">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="P21">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="9:16">
+      <c r="I22">
         <v>0.108</v>
       </c>
-      <c r="J21">
+      <c r="J22">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="K21">
+      <c r="K22">
         <v>0.17299999999999999</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>0.24099999999999999</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>2.4E-2</v>
       </c>
-      <c r="O21">
+      <c r="O22">
         <v>0.315</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>3.1E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Little bits of edits in Edinburgh
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19860" tabRatio="652" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="652" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="IRAS20050" sheetId="8" r:id="rId8"/>
     <sheet name="Oph_NGC1333" sheetId="9" r:id="rId9"/>
     <sheet name="OphNGC_fitted_params" sheetId="10" r:id="rId10"/>
+    <sheet name="IRAS20050params" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3508" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="382">
   <si>
     <t>\toprule</t>
   </si>
@@ -1182,8 +1183,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1234,7 +1235,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="595">
+  <cellStyleXfs count="627">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1830,8 +1831,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1843,12 +1876,13 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="595">
+  <cellStyles count="627">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2146,6 +2180,22 @@
     <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2443,6 +2493,22 @@
     <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3629,8 +3695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5848,6 +5914,629 @@
     </row>
     <row r="31" spans="1:26">
       <c r="A31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:V13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>349</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>350</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>378</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>381</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>185</v>
+      </c>
+      <c r="V3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>173</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>351</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>380</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>7.1313139999999997E-2</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0.74123358399999995</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="10">
+        <v>1.2070259999999999E-3</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M6" s="13">
+        <v>108.8000031</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O6" s="13">
+        <v>22.092800140000001</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>58.243137359999999</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="3">
+        <v>8</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.69999998799999996</v>
+      </c>
+      <c r="V6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.6492793960000001</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.77183942699999997</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.256000012</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.15896259200000001</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="13">
+        <v>39.899997710000001</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="13">
+        <v>9.4951848979999998</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>18.671718599999998</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="3">
+        <v>14</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.69999998799999996</v>
+      </c>
+      <c r="V7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.1346682640000001</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.73225057299999996</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.114</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="10">
+        <v>5.1234897000000001E-2</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="13">
+        <v>48.450000760000002</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8" s="13">
+        <v>9.8161163330000001</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>18.671718599999998</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="3">
+        <v>14</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1.1499999759999999</v>
+      </c>
+      <c r="V8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1.7117460980000001</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0.26631178900000002</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.577000022</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.41316226099999998</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="13">
+        <v>57</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O9" s="13">
+        <v>17.367547989999998</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>37.863647460000003</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="3">
+        <v>3</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.53666770399999997</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.78184027099999998</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="10">
+        <v>3.5247339999999999E-3</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="13">
+        <v>43.665500639999998</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O10" s="13">
+        <v>7.2344884870000001</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>46.826450350000002</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="3">
+        <v>13</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1.2999999520000001</v>
+      </c>
+      <c r="V10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10">
+        <v>-0.33831642200000001</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10">
+        <v>2.221856319</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="10">
+        <v>1.5022989999999999E-3</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="13">
+        <v>134.3999939</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="13">
+        <v>28.249481200000002</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>32.636898039999998</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" s="3">
+        <v>13</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.69999998799999996</v>
+      </c>
+      <c r="V11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1.294389333</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.4146896579999999</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="10">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.238314569</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" s="13">
+        <v>374.39999390000003</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O12" s="13">
+        <v>225.60357669999999</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>18.671718597400002</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" s="3">
+        <v>14</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1.2999999520000001</v>
+      </c>
+      <c r="V12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added lots of pictures, edited bits and pieces before 4th of July vacation
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="652" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20180" tabRatio="652" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Oph_NGC1333" sheetId="9" r:id="rId9"/>
     <sheet name="OphNGC_fitted_params" sheetId="10" r:id="rId10"/>
     <sheet name="IRAS20050params" sheetId="11" r:id="rId11"/>
+    <sheet name="NGC2071params" sheetId="12" r:id="rId12"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3634" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3783" uniqueCount="397">
   <si>
     <t>\toprule</t>
   </si>
@@ -1175,6 +1177,51 @@
   </si>
   <si>
     <t>$\Av$</t>
+  </si>
+  <si>
+    <t>\Ltot</t>
+  </si>
+  <si>
+    <t>05h47m04.8s +00d21m43.1s</t>
+  </si>
+  <si>
+    <t>05h47m04.7s +00d21m48.2s</t>
+  </si>
+  <si>
+    <t>05h47m05.4s +00d21m50.3s</t>
+  </si>
+  <si>
+    <t>05h47m04.0s +00d22m10.5s</t>
+  </si>
+  <si>
+    <t>05h47m10.7s +00d21m14.0s</t>
+  </si>
+  <si>
+    <t>\Lbol</t>
+  </si>
+  <si>
+    <t>S140</t>
+  </si>
+  <si>
+    <t>CepheusA</t>
+  </si>
+  <si>
+    <t>NGC2264</t>
+  </si>
+  <si>
+    <t>Ophiuchus</t>
+  </si>
+  <si>
+    <t>IRAS20050+2720</t>
+  </si>
+  <si>
+    <t>Cluster</t>
+  </si>
+  <si>
+    <t>\%</t>
+  </si>
+  <si>
+    <t>Fraction of time above \SI{10}{\degree} elevation</t>
   </si>
 </sst>
 </file>
@@ -1235,8 +1282,66 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="627">
+  <cellStyleXfs count="685">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1882,7 +1987,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="627">
+  <cellStyles count="685">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2196,6 +2301,35 @@
     <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2509,6 +2643,35 @@
     <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2841,7 +3004,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A7" sqref="A7:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5932,8 +6095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:U12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5980,19 +6143,19 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>349</v>
+        <v>158</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>350</v>
+        <v>382</v>
       </c>
       <c r="P3" t="s">
         <v>1</v>
       </c>
       <c r="Q3" t="s">
-        <v>378</v>
+        <v>184</v>
       </c>
       <c r="R3" t="s">
         <v>1</v>
@@ -6539,6 +6702,774 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:X12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:X12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="1:24">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>348</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>382</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>388</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>184</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>381</v>
+      </c>
+      <c r="V4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>185</v>
+      </c>
+      <c r="X4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>173</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>173</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>351</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>380</v>
+      </c>
+      <c r="V5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>383</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2.3091127249999999</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2.7841286169599999</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5">
+        <v>22.167999267599999</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="6">
+        <v>2.4184575080899999</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="11">
+        <v>49.399997711200001</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="11">
+        <v>4.4739060401900002</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>297.17919439299999</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="11">
+        <v>0</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>14</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="11">
+        <v>1.2999999523200001</v>
+      </c>
+      <c r="X7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2.2192471940999998</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1.82439509673</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5">
+        <v>6.5679998397799997</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1.71226215363</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="11">
+        <v>331.19998168900003</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O8" s="11">
+        <v>35.751724243200002</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>199.775606025</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11">
+        <v>18.671718597400002</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>14</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" s="11">
+        <v>1.2999999523200001</v>
+      </c>
+      <c r="X8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.0131348658099999</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2.2901173372399999</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>4.3790001869199999</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1.1248142719300001</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="11">
+        <v>374.39999389600001</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O9" s="11">
+        <v>48.687911987299998</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>113.72508824000001</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="11">
+        <v>18.671718597400002</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="11">
+        <v>1.2999999523200001</v>
+      </c>
+      <c r="X9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>386</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1.08106783233</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>3.96156284442</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="5">
+        <v>14.7790002823</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="6">
+        <v>5.2338862419099996</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="11">
+        <v>9.1999998092700004</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O10" s="11">
+        <v>2.1085712909700001</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>21.4463041182</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="11">
+        <v>0</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>14</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" s="11">
+        <v>1</v>
+      </c>
+      <c r="X10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>387</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.31504689430999999</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.0302400520199999</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1.49999996647E-2</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="6">
+        <v>6.7216595634800001E-3</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="11">
+        <v>22.099998474100001</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="11">
+        <v>6.2234702110300004</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>12.7304289238</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" s="11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>14</v>
+      </c>
+      <c r="V11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W11" s="11">
+        <v>1.2999999523200001</v>
+      </c>
+      <c r="X11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.5" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" t="s">
+        <v>389</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <f>K4*100</f>
+        <v>100</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="B5" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:F8" si="0">K5*100</f>
+        <v>95</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="B6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="B7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="B8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Edits while Lee and Stephen are reading
</commit_message>
<xml_diff>
--- a/Scripts/Tables.xlsx
+++ b/Scripts/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20180" tabRatio="652" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="1280" yWindow="0" windowWidth="38400" windowHeight="20580" tabRatio="652" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="OphNGC_fitted_params" sheetId="10" r:id="rId10"/>
     <sheet name="IRAS20050params" sheetId="11" r:id="rId11"/>
     <sheet name="NGC2071params" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet2" sheetId="13" r:id="rId13"/>
+    <sheet name="ObservingTimes" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3783" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3816" uniqueCount="402">
   <si>
     <t>\toprule</t>
   </si>
@@ -1080,12 +1080,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Env. Mass</t>
-  </si>
-  <si>
-    <t>Lum.</t>
-  </si>
-  <si>
     <t>\si{\degree}</t>
   </si>
   <si>
@@ -1167,9 +1161,6 @@
     <t>16h27m22s -24d29m54s</t>
   </si>
   <si>
-    <t>Inc.</t>
-  </si>
-  <si>
     <t>$\Lbol$</t>
   </si>
   <si>
@@ -1222,6 +1213,30 @@
   </si>
   <si>
     <t>Fraction of time above \SI{10}{\degree} elevation</t>
+  </si>
+  <si>
+    <t>$\Rfifty/\Rfifty_\textrm{cal}$</t>
+  </si>
+  <si>
+    <t>$R$</t>
+  </si>
+  <si>
+    <t>Calc. \Menv</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>(\si{\degree})</t>
+  </si>
+  <si>
+    <t>(\si{\Msun})</t>
+  </si>
+  <si>
+    <t>(mag)</t>
+  </si>
+  <si>
+    <t>(J2000)</t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1248,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1264,6 +1279,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1282,7 +1302,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="685">
+  <cellStyleXfs count="695">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1968,8 +1988,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1986,8 +2016,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="685">
+  <cellStyles count="695">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2330,6 +2363,11 @@
     <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="682" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2672,6 +2710,11 @@
     <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="681" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3856,20 +3899,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Z31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>347</v>
       </c>
@@ -3882,8 +3925,8 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>225</v>
+      <c r="E2" s="14" t="s">
+        <v>394</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -3895,54 +3938,60 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>348</v>
+        <v>395</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>349</v>
+        <v>158</v>
       </c>
       <c r="N2" t="s">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>350</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
+        <v>396</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>379</v>
       </c>
       <c r="T2" t="s">
         <v>1</v>
       </c>
       <c r="U2" t="s">
+        <v>376</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>397</v>
+      </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
         <v>378</v>
       </c>
-      <c r="V2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
-        <v>381</v>
-      </c>
-      <c r="X2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
         <v>185</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:28">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>401</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -3957,45 +4006,51 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>171</v>
+        <v>399</v>
       </c>
       <c r="N3" t="s">
         <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>173</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1</v>
-      </c>
-      <c r="S3" t="s">
-        <v>173</v>
+        <v>399</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>345</v>
       </c>
       <c r="T3" t="s">
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="V3" t="s">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="X3" t="s">
         <v>1</v>
       </c>
+      <c r="Y3" t="s">
+        <v>400</v>
+      </c>
       <c r="Z3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
         <v>263</v>
       </c>
@@ -4003,7 +4058,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -4038,44 +4093,50 @@
       <c r="N5" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="5">
+        <v>0.97246005237099997</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="11">
         <v>5.5999999046299997</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>82</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="S5" s="5">
         <v>3.12361049652</v>
       </c>
-      <c r="R5" t="s">
-        <v>1</v>
-      </c>
-      <c r="S5" s="5">
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5">
         <v>8.3845822239000007</v>
       </c>
-      <c r="T5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U5" s="11">
+      <c r="V5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" s="11">
         <v>0</v>
       </c>
-      <c r="V5" t="s">
-        <v>1</v>
-      </c>
-      <c r="W5">
+      <c r="X5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5">
         <v>12</v>
       </c>
-      <c r="X5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="5">
+      <c r="Z5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5">
         <v>0.85000002384200002</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -4083,7 +4144,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -4118,44 +4179,50 @@
       <c r="N6" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="5">
+        <v>0.44882771647899999</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="11">
         <v>5.5999999046299997</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>82</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>1.6915882825899999</v>
       </c>
-      <c r="R6" t="s">
-        <v>1</v>
-      </c>
-      <c r="S6" s="5">
+      <c r="T6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" s="5">
         <v>4.8222426513599999</v>
       </c>
-      <c r="T6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U6" s="11">
+      <c r="V6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V6" t="s">
-        <v>1</v>
-      </c>
-      <c r="W6">
+      <c r="X6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y6">
         <v>14</v>
       </c>
-      <c r="X6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="5">
+      <c r="Z6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
         <v>268</v>
       </c>
@@ -4163,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -4198,44 +4265,50 @@
       <c r="N7" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="5">
+        <v>0.26929662988699998</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11">
         <v>7.6999998092700004</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="S7" s="5">
         <v>1.37442851067</v>
       </c>
-      <c r="R7" t="s">
-        <v>1</v>
-      </c>
-      <c r="S7" s="5">
+      <c r="T7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5">
         <v>7.4687077439999996</v>
       </c>
-      <c r="T7" t="s">
-        <v>1</v>
-      </c>
-      <c r="U7" s="11">
+      <c r="V7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V7" t="s">
-        <v>1</v>
-      </c>
-      <c r="W7">
+      <c r="X7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7">
         <v>12</v>
       </c>
-      <c r="X7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="5">
+      <c r="Z7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
         <v>272</v>
       </c>
@@ -4243,7 +4316,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -4278,44 +4351,50 @@
       <c r="N8" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="5">
+        <v>1.1220692912000001</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="11">
         <v>3.5</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>82</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="S8" s="5">
         <v>0.79772979021099999</v>
       </c>
-      <c r="R8" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="5">
+      <c r="T8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5">
         <v>8.1042072520000001</v>
       </c>
-      <c r="T8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="11">
+      <c r="V8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" s="11">
         <v>0</v>
       </c>
-      <c r="V8" t="s">
-        <v>1</v>
-      </c>
-      <c r="W8">
+      <c r="X8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8">
         <v>14</v>
       </c>
-      <c r="X8" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="5">
+      <c r="Z8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:28">
       <c r="A9" t="s">
         <v>275</v>
       </c>
@@ -4323,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -4358,44 +4437,50 @@
       <c r="N9" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="5">
+        <v>1.4960923882599999</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="11">
         <v>2.83050012589</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>82</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="S9" s="5">
         <v>0.419591218233</v>
       </c>
-      <c r="R9" t="s">
-        <v>1</v>
-      </c>
-      <c r="S9" s="5">
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="5">
         <v>3.05583030322</v>
       </c>
-      <c r="T9" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" s="11">
+      <c r="V9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V9" t="s">
-        <v>1</v>
-      </c>
-      <c r="W9">
+      <c r="X9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9">
         <v>14</v>
       </c>
-      <c r="X9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>1</v>
-      </c>
       <c r="Z9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:28">
       <c r="A10" t="s">
         <v>278</v>
       </c>
@@ -4403,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -4438,44 +4523,50 @@
       <c r="N10" t="s">
         <v>1</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="5">
+        <v>1.4960923882599999</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="11">
         <v>2.88599991798</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>82</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="S10" s="5">
         <v>1.00030839443</v>
       </c>
-      <c r="R10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S10" s="5">
+      <c r="T10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" s="5">
         <v>2.78605885712</v>
       </c>
-      <c r="T10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U10" s="11">
+      <c r="V10" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W10">
+      <c r="X10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10">
         <v>9</v>
       </c>
-      <c r="X10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="5">
+      <c r="Z10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AB10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:28">
       <c r="A11" t="s">
         <v>281</v>
       </c>
@@ -4483,7 +4574,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -4518,44 +4609,50 @@
       <c r="N11" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="5">
+        <v>0.47126910230300001</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="11">
         <v>4.25</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>82</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="S11" s="5">
         <v>1.7153609991100001</v>
       </c>
-      <c r="R11" t="s">
-        <v>1</v>
-      </c>
-      <c r="S11" s="5">
+      <c r="T11" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" s="5">
         <v>1.15500812031</v>
       </c>
-      <c r="T11" t="s">
-        <v>1</v>
-      </c>
-      <c r="U11" s="11">
+      <c r="V11" t="s">
+        <v>1</v>
+      </c>
+      <c r="W11" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V11" t="s">
-        <v>1</v>
-      </c>
-      <c r="W11">
+      <c r="X11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11">
         <v>14</v>
       </c>
-      <c r="X11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="5">
-        <v>1</v>
-      </c>
       <c r="Z11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:28">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -4563,7 +4660,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
@@ -4598,44 +4695,50 @@
       <c r="N12" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="11">
         <v>9.5625</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>82</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="S12" s="5">
         <v>2.1621778011299999</v>
       </c>
-      <c r="R12" t="s">
-        <v>1</v>
-      </c>
-      <c r="S12" s="5">
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" s="5">
         <v>1.3566864974899999</v>
       </c>
-      <c r="T12" t="s">
-        <v>1</v>
-      </c>
-      <c r="U12" s="11">
+      <c r="V12" t="s">
+        <v>1</v>
+      </c>
+      <c r="W12" s="11">
         <v>50.833290100100001</v>
       </c>
-      <c r="V12" t="s">
-        <v>1</v>
-      </c>
-      <c r="W12">
+      <c r="X12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12">
         <v>0</v>
       </c>
-      <c r="X12" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="5">
+      <c r="Z12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AB12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:28">
       <c r="A13" t="s">
         <v>285</v>
       </c>
@@ -4643,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -4678,44 +4781,50 @@
       <c r="N13" t="s">
         <v>1</v>
       </c>
-      <c r="O13" s="11">
+      <c r="O13" s="5">
+        <v>2.01972472416</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="11">
         <v>14.2999992371</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>82</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="S13" s="5">
         <v>2.2378678321800001</v>
       </c>
-      <c r="R13" t="s">
-        <v>1</v>
-      </c>
-      <c r="S13" s="5">
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" s="5">
         <v>35.106406334799999</v>
       </c>
-      <c r="T13" t="s">
-        <v>1</v>
-      </c>
-      <c r="U13" s="11">
+      <c r="V13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W13" s="11">
         <v>0</v>
       </c>
-      <c r="V13" t="s">
-        <v>1</v>
-      </c>
-      <c r="W13">
+      <c r="X13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13">
         <v>12</v>
       </c>
-      <c r="X13" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="5">
+      <c r="Z13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AB13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:28">
       <c r="A14" t="s">
         <v>286</v>
       </c>
@@ -4723,7 +4832,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -4758,44 +4867,50 @@
       <c r="N14" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="5">
+        <v>1.7205062465000001</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="11">
         <v>19.5499992371</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>82</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="S14" s="5">
         <v>3.6712670326199999</v>
       </c>
-      <c r="R14" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="5">
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="5">
         <v>24.282984853399999</v>
       </c>
-      <c r="T14" t="s">
-        <v>1</v>
-      </c>
-      <c r="U14" s="11">
+      <c r="V14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V14" t="s">
-        <v>1</v>
-      </c>
-      <c r="W14">
+      <c r="X14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14">
         <v>14</v>
       </c>
-      <c r="X14" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="5">
+      <c r="Z14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AB14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:28">
       <c r="A15" t="s">
         <v>287</v>
       </c>
@@ -4803,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -4838,44 +4953,50 @@
       <c r="N15" t="s">
         <v>1</v>
       </c>
-      <c r="O15" s="11">
+      <c r="O15" s="5">
+        <v>4.0477753442100001E-2</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="11">
         <v>9.5625</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>82</v>
       </c>
-      <c r="Q15" s="5">
+      <c r="S15" s="5">
         <v>1.7964602708799999</v>
       </c>
-      <c r="R15" t="s">
-        <v>1</v>
-      </c>
-      <c r="S15" s="5">
+      <c r="T15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="5">
         <v>3.6267898991499998</v>
       </c>
-      <c r="T15" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" s="11">
+      <c r="V15" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="11">
         <v>65.098937988299994</v>
       </c>
-      <c r="V15" t="s">
-        <v>1</v>
-      </c>
-      <c r="W15">
+      <c r="X15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15">
         <v>4</v>
       </c>
-      <c r="X15" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="5">
+      <c r="Z15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AB15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:28">
       <c r="A16" t="s">
         <v>290</v>
       </c>
@@ -4883,7 +5004,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -4918,44 +5039,50 @@
       <c r="N16" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="5">
+        <v>4.2608161518100001E-3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="11">
         <v>1.9239999055899999</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>82</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="S16" s="5">
         <v>0.379579424858</v>
       </c>
-      <c r="R16" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" s="5">
+      <c r="T16" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" s="5">
         <v>0.54861610563300001</v>
       </c>
-      <c r="T16" t="s">
-        <v>1</v>
-      </c>
-      <c r="U16" s="11">
+      <c r="V16" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" s="11">
         <v>61.726287841800001</v>
       </c>
-      <c r="V16" t="s">
-        <v>1</v>
-      </c>
-      <c r="W16">
+      <c r="X16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y16">
         <v>14</v>
       </c>
-      <c r="X16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="5">
+      <c r="Z16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="5">
         <v>1.1499999761599999</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AB16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:28">
       <c r="A17" t="s">
         <v>299</v>
       </c>
@@ -4963,7 +5090,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -4998,44 +5125,50 @@
       <c r="N17" t="s">
         <v>1</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="5">
+        <v>8.5216323036099995E-3</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="11">
         <v>6.5</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>82</v>
       </c>
-      <c r="Q17" s="5">
+      <c r="S17" s="5">
         <v>1.6256260871899999</v>
       </c>
-      <c r="R17" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="5">
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" s="5">
         <v>1.49126920974</v>
       </c>
-      <c r="T17" t="s">
-        <v>1</v>
-      </c>
-      <c r="U17" s="11">
+      <c r="V17" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="11">
         <v>65.098937988299994</v>
       </c>
-      <c r="V17" t="s">
-        <v>1</v>
-      </c>
-      <c r="W17">
+      <c r="X17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17">
         <v>14</v>
       </c>
-      <c r="X17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="5">
+      <c r="Z17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z17" t="s">
+      <c r="AB17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:28">
       <c r="A18" t="s">
         <v>302</v>
       </c>
@@ -5043,7 +5176,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -5078,44 +5211,50 @@
       <c r="N18" t="s">
         <v>1</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="5">
+        <v>2.1304080759000001E-2</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="11">
         <v>2.88599991798</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>82</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="S18" s="5">
         <v>0.77512139081999998</v>
       </c>
-      <c r="R18" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="5">
+      <c r="T18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" s="5">
         <v>0.95077358247199995</v>
       </c>
-      <c r="T18" t="s">
-        <v>1</v>
-      </c>
-      <c r="U18" s="11">
+      <c r="V18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" s="11">
         <v>18.671718597400002</v>
       </c>
-      <c r="V18" t="s">
-        <v>1</v>
-      </c>
-      <c r="W18">
+      <c r="X18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18">
         <v>14</v>
       </c>
-      <c r="X18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="5">
+      <c r="Z18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AB18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="1:28">
       <c r="A19" t="s">
         <v>305</v>
       </c>
@@ -5123,7 +5262,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
@@ -5158,44 +5297,50 @@
       <c r="N19" t="s">
         <v>1</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="5">
+        <v>1.9173672683099999E-2</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="11">
         <v>2.83050012589</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="S19" s="5">
         <v>0.58911883831</v>
       </c>
-      <c r="R19" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="5">
+      <c r="T19" t="s">
+        <v>1</v>
+      </c>
+      <c r="U19" s="5">
         <v>0.55470980600800002</v>
       </c>
-      <c r="T19" t="s">
-        <v>1</v>
-      </c>
-      <c r="U19" s="11">
+      <c r="V19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" s="11">
         <v>54.623458862299998</v>
       </c>
-      <c r="V19" t="s">
-        <v>1</v>
-      </c>
-      <c r="W19">
+      <c r="X19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19">
         <v>12</v>
       </c>
-      <c r="X19" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="5">
+      <c r="Z19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AB19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>308</v>
       </c>
@@ -5203,7 +5348,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
@@ -5238,44 +5383,50 @@
       <c r="N20" t="s">
         <v>1</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O20" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="11">
         <v>17.716999053999999</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>82</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="S20" s="5">
         <v>4.6975569725000001</v>
       </c>
-      <c r="R20" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" s="5">
+      <c r="T20" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" s="5">
         <v>1.6559064728899999</v>
       </c>
-      <c r="T20" t="s">
-        <v>1</v>
-      </c>
-      <c r="U20" s="11">
+      <c r="V20" t="s">
+        <v>1</v>
+      </c>
+      <c r="W20" s="11">
         <v>74.742477417000003</v>
       </c>
-      <c r="V20" t="s">
-        <v>1</v>
-      </c>
-      <c r="W20">
+      <c r="X20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y20">
         <v>9</v>
       </c>
-      <c r="X20" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="5">
+      <c r="Z20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AB20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>311</v>
       </c>
@@ -5283,7 +5434,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -5318,44 +5469,50 @@
       <c r="N21" t="s">
         <v>1</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="11">
         <v>4.25</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>82</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="S21" s="5">
         <v>0.87547254562400001</v>
       </c>
-      <c r="R21" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" s="5">
+      <c r="T21" t="s">
+        <v>1</v>
+      </c>
+      <c r="U21" s="5">
         <v>0.62906498693500001</v>
       </c>
-      <c r="T21" t="s">
-        <v>1</v>
-      </c>
-      <c r="U21" s="11">
+      <c r="V21" t="s">
+        <v>1</v>
+      </c>
+      <c r="W21" s="11">
         <v>77.846801757799994</v>
       </c>
-      <c r="V21" t="s">
-        <v>1</v>
-      </c>
-      <c r="W21">
+      <c r="X21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21">
         <v>14</v>
       </c>
-      <c r="X21" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="5">
+      <c r="Z21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AB21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="1:28">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -5363,7 +5520,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -5398,44 +5555,50 @@
       <c r="N22" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="11">
+      <c r="O22" s="5">
+        <v>3.6216937290299997E-2</v>
+      </c>
+      <c r="P22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="11">
         <v>1.25800001621</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>82</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="S22" s="5">
         <v>0.21417433023499999</v>
       </c>
-      <c r="R22" t="s">
-        <v>1</v>
-      </c>
-      <c r="S22" s="5">
+      <c r="T22" t="s">
+        <v>1</v>
+      </c>
+      <c r="U22" s="5">
         <v>0.22290228130799999</v>
       </c>
-      <c r="T22" t="s">
-        <v>1</v>
-      </c>
-      <c r="U22" s="11">
+      <c r="V22" t="s">
+        <v>1</v>
+      </c>
+      <c r="W22" s="11">
         <v>65.098937988299994</v>
       </c>
-      <c r="V22" t="s">
-        <v>1</v>
-      </c>
-      <c r="W22">
+      <c r="X22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y22">
         <v>14</v>
       </c>
-      <c r="X22" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="5">
+      <c r="Z22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AB22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="1:28">
       <c r="A23" t="s">
         <v>317</v>
       </c>
@@ -5443,7 +5606,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -5478,44 +5641,50 @@
       <c r="N23" t="s">
         <v>1</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O23" s="5">
+        <v>8.5216323036099995E-3</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="11">
         <v>3.5</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>82</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="S23" s="5">
         <v>0.74467575550099996</v>
       </c>
-      <c r="R23" t="s">
-        <v>1</v>
-      </c>
-      <c r="S23" s="5">
+      <c r="T23" t="s">
+        <v>1</v>
+      </c>
+      <c r="U23" s="5">
         <v>1.09769474728</v>
       </c>
-      <c r="T23" t="s">
-        <v>1</v>
-      </c>
-      <c r="U23" s="11">
+      <c r="V23" t="s">
+        <v>1</v>
+      </c>
+      <c r="W23" s="11">
         <v>58.243137359599999</v>
       </c>
-      <c r="V23" t="s">
-        <v>1</v>
-      </c>
-      <c r="W23">
+      <c r="X23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y23">
         <v>13</v>
       </c>
-      <c r="X23" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="5">
+      <c r="Z23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="AB23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="1:28">
       <c r="A24" t="s">
         <v>320</v>
       </c>
@@ -5523,7 +5692,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
@@ -5558,44 +5727,50 @@
       <c r="N24" t="s">
         <v>1</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="5">
+        <v>5.1129793821699999E-2</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="11">
         <v>5</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>82</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="S24" s="5">
         <v>0.97076719999299999</v>
       </c>
-      <c r="R24" t="s">
-        <v>1</v>
-      </c>
-      <c r="S24" s="5">
+      <c r="T24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U24" s="5">
         <v>1.1900235692700001</v>
       </c>
-      <c r="T24" t="s">
-        <v>1</v>
-      </c>
-      <c r="U24" s="11">
+      <c r="V24" t="s">
+        <v>1</v>
+      </c>
+      <c r="W24" s="11">
         <v>77.846801757799994</v>
       </c>
-      <c r="V24" t="s">
-        <v>1</v>
-      </c>
-      <c r="W24">
+      <c r="X24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24">
         <v>14</v>
       </c>
-      <c r="X24" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="5">
-        <v>1</v>
-      </c>
       <c r="Z24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="1:28">
       <c r="A25" t="s">
         <v>323</v>
       </c>
@@ -5603,7 +5778,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
@@ -5638,44 +5813,50 @@
       <c r="N25" t="s">
         <v>1</v>
       </c>
-      <c r="O25" s="11">
+      <c r="O25" s="5">
+        <v>4.0477753442100001E-2</v>
+      </c>
+      <c r="P25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="11">
         <v>59.5</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>82</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="S25" s="5">
         <v>11.989372253399999</v>
       </c>
-      <c r="R25" t="s">
-        <v>1</v>
-      </c>
-      <c r="S25" s="5">
+      <c r="T25" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" s="5">
         <v>13.392611267099999</v>
       </c>
-      <c r="T25" t="s">
-        <v>1</v>
-      </c>
-      <c r="U25" s="11">
+      <c r="V25" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" s="11">
         <v>37.863647460899998</v>
       </c>
-      <c r="V25" t="s">
-        <v>1</v>
-      </c>
-      <c r="W25">
+      <c r="X25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y25">
         <v>10</v>
       </c>
-      <c r="X25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="5">
+      <c r="Z25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="AB25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="1:28">
       <c r="A26" t="s">
         <v>329</v>
       </c>
@@ -5683,7 +5864,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
@@ -5718,44 +5899,50 @@
       <c r="N26" t="s">
         <v>1</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="5">
+        <v>3.19561211385E-2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="11">
         <v>2.88599991798</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>82</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="S26" s="5">
         <v>0.65629565715799998</v>
       </c>
-      <c r="R26" t="s">
-        <v>1</v>
-      </c>
-      <c r="S26" s="5">
+      <c r="T26" t="s">
+        <v>1</v>
+      </c>
+      <c r="U26" s="5">
         <v>0.53428820958000001</v>
       </c>
-      <c r="T26" t="s">
-        <v>1</v>
-      </c>
-      <c r="U26" s="11">
+      <c r="V26" t="s">
+        <v>1</v>
+      </c>
+      <c r="W26" s="11">
         <v>68.381729125999996</v>
       </c>
-      <c r="V26" t="s">
-        <v>1</v>
-      </c>
-      <c r="W26">
+      <c r="X26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y26">
         <v>14</v>
       </c>
-      <c r="X26" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="5">
+      <c r="Z26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="5">
         <v>1.2999999523200001</v>
       </c>
-      <c r="Z26" t="s">
+      <c r="AB26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="1:28">
       <c r="A27" t="s">
         <v>332</v>
       </c>
@@ -5763,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -5798,44 +5985,50 @@
       <c r="N27" t="s">
         <v>1</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="5">
+        <v>2.00258359135E-2</v>
+      </c>
+      <c r="P27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="11">
         <v>9.5625</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>82</v>
       </c>
-      <c r="Q27" s="5">
+      <c r="S27" s="5">
         <v>3.4096145629899999</v>
       </c>
-      <c r="R27" t="s">
-        <v>1</v>
-      </c>
-      <c r="S27" s="5">
+      <c r="T27" t="s">
+        <v>1</v>
+      </c>
+      <c r="U27" s="5">
         <v>0.73242401538599999</v>
       </c>
-      <c r="T27" t="s">
-        <v>1</v>
-      </c>
-      <c r="U27" s="11">
+      <c r="V27" t="s">
+        <v>1</v>
+      </c>
+      <c r="W27" s="11">
         <v>90</v>
       </c>
-      <c r="V27" t="s">
-        <v>1</v>
-      </c>
-      <c r="W27">
+      <c r="X27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y27">
         <v>12</v>
       </c>
-      <c r="X27" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="5">
+      <c r="Z27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AB27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="1:28">
       <c r="A28" t="s">
         <v>335</v>
       </c>
@@ -5843,7 +6036,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
@@ -5878,44 +6071,50 @@
       <c r="N28" t="s">
         <v>1</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="5">
+        <v>2.5564896910800002E-2</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="11">
         <v>26.600000381499999</v>
       </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
         <v>82</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="S28" s="5">
         <v>4.9007120132399997</v>
       </c>
-      <c r="R28" t="s">
-        <v>1</v>
-      </c>
-      <c r="S28" s="5">
+      <c r="T28" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="5">
         <v>6.4723829178900001</v>
       </c>
-      <c r="T28" t="s">
-        <v>1</v>
-      </c>
-      <c r="U28" s="11">
+      <c r="V28" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" s="11">
         <v>74.742477417000003</v>
       </c>
-      <c r="V28" t="s">
-        <v>1</v>
-      </c>
-      <c r="W28">
+      <c r="X28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y28">
         <v>14</v>
       </c>
-      <c r="X28" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="5">
+      <c r="Z28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="AB28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="1:28">
       <c r="A29" t="s">
         <v>338</v>
       </c>
@@ -5923,7 +6122,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
@@ -5958,44 +6157,50 @@
       <c r="N29" t="s">
         <v>1</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="5">
+        <v>2.5564896910800002E-2</v>
+      </c>
+      <c r="P29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="11">
         <v>26.579000473000001</v>
       </c>
-      <c r="P29" t="s">
+      <c r="R29" t="s">
         <v>82</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="S29" s="5">
         <v>5.1450510024999998</v>
       </c>
-      <c r="R29" t="s">
-        <v>1</v>
-      </c>
-      <c r="S29" s="5">
+      <c r="T29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U29" s="5">
         <v>5.0039232296899998</v>
       </c>
-      <c r="T29" t="s">
-        <v>1</v>
-      </c>
-      <c r="U29" s="11">
+      <c r="V29" t="s">
+        <v>1</v>
+      </c>
+      <c r="W29" s="11">
         <v>80.915283203100003</v>
       </c>
-      <c r="V29" t="s">
-        <v>1</v>
-      </c>
-      <c r="W29">
+      <c r="X29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y29">
         <v>14</v>
       </c>
-      <c r="X29" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="5">
+      <c r="Z29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="AB29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="1:28">
       <c r="A30" t="s">
         <v>341</v>
       </c>
@@ -6003,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
@@ -6038,44 +6243,50 @@
       <c r="N30" t="s">
         <v>1</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="5">
+        <v>8.5216323036099995E-3</v>
+      </c>
+      <c r="P30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="11">
         <v>11.8159990311</v>
       </c>
-      <c r="P30" t="s">
+      <c r="R30" t="s">
         <v>82</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="S30" s="5">
         <v>2.71168518066</v>
       </c>
-      <c r="R30" t="s">
-        <v>1</v>
-      </c>
-      <c r="S30" s="5">
+      <c r="T30" t="s">
+        <v>1</v>
+      </c>
+      <c r="U30" s="5">
         <v>0.99068716077300001</v>
       </c>
-      <c r="T30" t="s">
-        <v>1</v>
-      </c>
-      <c r="U30" s="11">
+      <c r="V30" t="s">
+        <v>1</v>
+      </c>
+      <c r="W30" s="11">
         <v>80.915283203100003</v>
       </c>
-      <c r="V30" t="s">
-        <v>1</v>
-      </c>
-      <c r="W30">
+      <c r="X30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y30">
         <v>14</v>
       </c>
-      <c r="X30" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y30" s="5">
+      <c r="Z30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA30" s="5">
         <v>0.69999998807899999</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AB30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="1:28">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -6149,7 +6360,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="P3" t="s">
         <v>1</v>
@@ -6161,7 +6372,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="T3" t="s">
         <v>1</v>
@@ -6202,13 +6413,13 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="R4" t="s">
         <v>1</v>
       </c>
       <c r="S4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="T4" t="s">
         <v>1</v>
@@ -6761,13 +6972,13 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="P4" t="s">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="R4" t="s">
         <v>1</v>
@@ -6779,7 +6990,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="V4" t="s">
         <v>1</v>
@@ -6826,13 +7037,13 @@
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="T5" t="s">
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="V5" t="s">
         <v>1</v>
@@ -6854,7 +7065,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -6928,7 +7139,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -7002,7 +7213,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -7076,7 +7287,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -7150,7 +7361,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
@@ -7236,7 +7447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
@@ -7255,7 +7466,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="B2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -7267,7 +7478,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H2" t="s">
         <v>40</v>
@@ -7283,7 +7494,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="B4" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -7299,7 +7510,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H4" t="s">
         <v>40</v>
@@ -7310,7 +7521,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="B5" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -7326,7 +7537,7 @@
         <v>95</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H5" t="s">
         <v>40</v>
@@ -7337,7 +7548,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="B6" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -7353,7 +7564,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H6" t="s">
         <v>40</v>
@@ -7364,7 +7575,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="B7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -7380,7 +7591,7 @@
         <v>80</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H7" t="s">
         <v>40</v>
@@ -7391,7 +7602,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="B8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -7407,7 +7618,7 @@
         <v>70</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H8" t="s">
         <v>40</v>
@@ -14248,7 +14459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CU94"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>

</xml_diff>